<commit_message>
Made some overview and hormonized the different soil ID from SUA and USDM.
</commit_message>
<xml_diff>
--- a/Termites/Soil_Data.xlsx
+++ b/Termites/Soil_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansun\Google Drive\Skole\Master\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansun\Documents\Master\GitHub__R-stat\AfricanBioServices-Vegetation-and-soils\Termites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9695DBCD-2C50-4A4C-90A5-A3F2B38DB338}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5C0E2137-9A01-4A9E-9420-54522CE53A8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUAsoil" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="USDMSoil" sheetId="4" r:id="rId3"/>
     <sheet name="SUAvsUSDM" sheetId="5" r:id="rId4"/>
     <sheet name="List of blocks" sheetId="6" r:id="rId5"/>
+    <sheet name="Ark1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="224">
   <si>
     <t>S/N</t>
   </si>
@@ -787,6 +788,30 @@
   </si>
   <si>
     <t>List of the blocks I should have samples from:</t>
+  </si>
+  <si>
+    <t>CLUMPY</t>
+  </si>
+  <si>
+    <t>FINE</t>
+  </si>
+  <si>
+    <t>GRAINED</t>
+  </si>
+  <si>
+    <t>Samples sent with Marit</t>
+  </si>
+  <si>
+    <t>31.2.2017</t>
+  </si>
+  <si>
+    <t>Samples sent with Vilde</t>
+  </si>
+  <si>
+    <t>Makao</t>
+  </si>
+  <si>
+    <t>gram sent</t>
   </si>
 </sst>
 </file>
@@ -1516,12 +1541,6 @@
     <xf numFmtId="0" fontId="32" fillId="31" borderId="0" xfId="47"/>
     <xf numFmtId="14" fontId="32" fillId="31" borderId="0" xfId="47" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="46" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1558,26 +1577,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="46"/>
     <xf numFmtId="0" fontId="36" fillId="26" borderId="0" xfId="46" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="30" fillId="28" borderId="0" xfId="45" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="30" fillId="28" borderId="0" xfId="45" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="46" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="26" borderId="0" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="26" borderId="0" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="46" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -1942,8 +1967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L99" sqref="L99"/>
+    <sheetView topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1951,7 +1976,7 @@
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
     <col min="2" max="4" width="19.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="18" style="54" customWidth="1"/>
+    <col min="6" max="6" width="18" style="52" customWidth="1"/>
     <col min="7" max="7" width="9.109375" style="18" customWidth="1"/>
     <col min="8" max="14" width="8.88671875" customWidth="1"/>
     <col min="15" max="15" width="12.88671875" customWidth="1"/>
@@ -3016,7 +3041,7 @@
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="52" t="s">
+      <c r="E59" s="50" t="s">
         <v>165</v>
       </c>
       <c r="F59" s="34" t="s">
@@ -3035,7 +3060,7 @@
       <c r="E60" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F60" s="53">
+      <c r="F60" s="51">
         <v>2</v>
       </c>
       <c r="G60" s="14">
@@ -3053,7 +3078,7 @@
       <c r="E61" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F61" s="53">
+      <c r="F61" s="51">
         <v>2</v>
       </c>
       <c r="G61" s="14">
@@ -3073,7 +3098,7 @@
       <c r="E62" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F62" s="53">
+      <c r="F62" s="51">
         <v>2</v>
       </c>
       <c r="G62" s="14">
@@ -3091,7 +3116,7 @@
       <c r="E63" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F63" s="53">
+      <c r="F63" s="51">
         <v>2</v>
       </c>
       <c r="G63" s="14">
@@ -3109,7 +3134,7 @@
       <c r="E64" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F64" s="53">
+      <c r="F64" s="51">
         <v>2</v>
       </c>
       <c r="G64" s="14">
@@ -3127,7 +3152,7 @@
       <c r="E65" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="53">
+      <c r="F65" s="51">
         <v>2</v>
       </c>
       <c r="G65" s="14">
@@ -3145,7 +3170,7 @@
       <c r="E66" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F66" s="53">
+      <c r="F66" s="51">
         <v>2</v>
       </c>
       <c r="G66" s="14">
@@ -3163,7 +3188,7 @@
       <c r="E67" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F67" s="53">
+      <c r="F67" s="51">
         <v>2</v>
       </c>
       <c r="G67" s="14">
@@ -3181,7 +3206,7 @@
       <c r="E68" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="53">
+      <c r="F68" s="51">
         <v>2</v>
       </c>
       <c r="G68" s="14">
@@ -3199,7 +3224,7 @@
       <c r="E69" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F69" s="53">
+      <c r="F69" s="51">
         <v>2</v>
       </c>
       <c r="G69" s="14">
@@ -3219,7 +3244,7 @@
       <c r="E70" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F70" s="53">
+      <c r="F70" s="51">
         <v>2</v>
       </c>
       <c r="G70" s="14">
@@ -3237,7 +3262,7 @@
       <c r="E71" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F71" s="53">
+      <c r="F71" s="51">
         <v>2</v>
       </c>
       <c r="G71" s="14">
@@ -3255,7 +3280,7 @@
       <c r="E72" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F72" s="53">
+      <c r="F72" s="51">
         <v>2</v>
       </c>
       <c r="G72" s="14">
@@ -3273,7 +3298,7 @@
       <c r="E73" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F73" s="53">
+      <c r="F73" s="51">
         <v>2</v>
       </c>
       <c r="G73" s="14">
@@ -3291,7 +3316,7 @@
       <c r="E74" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F74" s="53">
+      <c r="F74" s="51">
         <v>2</v>
       </c>
       <c r="G74" s="14">
@@ -3309,7 +3334,7 @@
       <c r="E75" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F75" s="53">
+      <c r="F75" s="51">
         <v>2</v>
       </c>
       <c r="G75" s="14">
@@ -3327,7 +3352,7 @@
       <c r="E76" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F76" s="53">
+      <c r="F76" s="51">
         <v>2</v>
       </c>
       <c r="G76" s="14">
@@ -3345,7 +3370,7 @@
       <c r="E77" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F77" s="53">
+      <c r="F77" s="51">
         <v>2</v>
       </c>
       <c r="G77" s="14">
@@ -3363,7 +3388,7 @@
       <c r="E78" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F78" s="53">
+      <c r="F78" s="51">
         <v>2</v>
       </c>
       <c r="G78" s="14">
@@ -3381,7 +3406,7 @@
       <c r="E79" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F79" s="53">
+      <c r="F79" s="51">
         <v>2</v>
       </c>
       <c r="G79" s="14">
@@ -3401,7 +3426,7 @@
       <c r="E80" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F80" s="53">
+      <c r="F80" s="51">
         <v>2</v>
       </c>
       <c r="G80" s="14">
@@ -3421,7 +3446,7 @@
       <c r="E81" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F81" s="53">
+      <c r="F81" s="51">
         <v>2</v>
       </c>
       <c r="G81" s="14">
@@ -3439,7 +3464,7 @@
       <c r="E82" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F82" s="53">
+      <c r="F82" s="51">
         <v>2</v>
       </c>
       <c r="G82" s="14">
@@ -3457,7 +3482,7 @@
       <c r="E83" s="26">
         <v>42796</v>
       </c>
-      <c r="F83" s="54">
+      <c r="F83" s="52">
         <v>1</v>
       </c>
       <c r="G83" s="14">
@@ -3475,7 +3500,7 @@
       <c r="E84" s="26">
         <v>42796</v>
       </c>
-      <c r="F84" s="54">
+      <c r="F84" s="52">
         <v>1</v>
       </c>
       <c r="G84" s="14">
@@ -3493,7 +3518,7 @@
       <c r="E85" s="26">
         <v>42796</v>
       </c>
-      <c r="F85" s="54">
+      <c r="F85" s="52">
         <v>1</v>
       </c>
       <c r="G85" s="14">
@@ -3513,7 +3538,7 @@
       <c r="E86" s="27">
         <v>42796</v>
       </c>
-      <c r="F86" s="55">
+      <c r="F86" s="53">
         <v>1</v>
       </c>
       <c r="G86" s="14">
@@ -3531,7 +3556,7 @@
       <c r="E87" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F87" s="54">
+      <c r="F87" s="52">
         <v>2</v>
       </c>
       <c r="G87" s="14">
@@ -3549,7 +3574,7 @@
       <c r="E88" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F88" s="54">
+      <c r="F88" s="52">
         <v>2</v>
       </c>
       <c r="G88" s="14">
@@ -3567,7 +3592,7 @@
       <c r="E89" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F89" s="54">
+      <c r="F89" s="52">
         <v>2</v>
       </c>
       <c r="G89" s="14">
@@ -3585,7 +3610,7 @@
       <c r="E90" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F90" s="54">
+      <c r="F90" s="52">
         <v>2</v>
       </c>
       <c r="G90" s="14">
@@ -3603,7 +3628,7 @@
       <c r="E91" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F91" s="54">
+      <c r="F91" s="52">
         <v>1</v>
       </c>
       <c r="G91" s="14">
@@ -3621,7 +3646,7 @@
       <c r="E92" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F92" s="54">
+      <c r="F92" s="52">
         <v>1</v>
       </c>
       <c r="G92" s="14">
@@ -3639,7 +3664,7 @@
       <c r="E93" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F93" s="54">
+      <c r="F93" s="52">
         <v>1</v>
       </c>
       <c r="G93" s="14">
@@ -3657,7 +3682,7 @@
       <c r="E94" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F94" s="54">
+      <c r="F94" s="52">
         <v>1</v>
       </c>
       <c r="G94" s="14">
@@ -3675,7 +3700,7 @@
       <c r="E95" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F95" s="54">
+      <c r="F95" s="52">
         <v>1</v>
       </c>
       <c r="G95" s="14">
@@ -3693,7 +3718,7 @@
       <c r="E96" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F96" s="54">
+      <c r="F96" s="52">
         <v>1</v>
       </c>
       <c r="G96" s="14">
@@ -3711,7 +3736,7 @@
       <c r="E97" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F97" s="54">
+      <c r="F97" s="52">
         <v>1</v>
       </c>
       <c r="G97" s="14">
@@ -3729,7 +3754,7 @@
       <c r="E98" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F98" s="54">
+      <c r="F98" s="52">
         <v>1</v>
       </c>
       <c r="G98" s="14">
@@ -3747,7 +3772,7 @@
       <c r="E99" s="26">
         <v>42737</v>
       </c>
-      <c r="F99" s="54">
+      <c r="F99" s="52">
         <v>1</v>
       </c>
       <c r="G99" s="14">
@@ -3765,7 +3790,7 @@
       <c r="E100" s="26">
         <v>42737</v>
       </c>
-      <c r="F100" s="54">
+      <c r="F100" s="52">
         <v>1</v>
       </c>
       <c r="G100" s="14">
@@ -3783,7 +3808,7 @@
       <c r="E101" s="26">
         <v>42737</v>
       </c>
-      <c r="F101" s="54">
+      <c r="F101" s="52">
         <v>1</v>
       </c>
       <c r="G101" s="14">
@@ -3801,7 +3826,7 @@
       <c r="E102" s="26">
         <v>42737</v>
       </c>
-      <c r="F102" s="54">
+      <c r="F102" s="52">
         <v>1</v>
       </c>
       <c r="G102" s="14">
@@ -3819,7 +3844,7 @@
       <c r="E103" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F103" s="54">
+      <c r="F103" s="52">
         <v>1</v>
       </c>
       <c r="G103" s="14">
@@ -3837,7 +3862,7 @@
       <c r="E104" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F104" s="54">
+      <c r="F104" s="52">
         <v>1</v>
       </c>
       <c r="G104" s="14">
@@ -3855,7 +3880,7 @@
       <c r="E105" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F105" s="54">
+      <c r="F105" s="52">
         <v>1</v>
       </c>
       <c r="G105" s="14">
@@ -3873,7 +3898,7 @@
       <c r="E106" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F106" s="54">
+      <c r="F106" s="52">
         <v>1</v>
       </c>
       <c r="G106" s="14">
@@ -3891,7 +3916,7 @@
       <c r="E107" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F107" s="54">
+      <c r="F107" s="52">
         <v>1</v>
       </c>
       <c r="G107" s="14">
@@ -3909,7 +3934,7 @@
       <c r="E108" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F108" s="54">
+      <c r="F108" s="52">
         <v>1</v>
       </c>
       <c r="G108" s="14">
@@ -3927,7 +3952,7 @@
       <c r="E109" s="26">
         <v>42737</v>
       </c>
-      <c r="F109" s="54">
+      <c r="F109" s="52">
         <v>1</v>
       </c>
       <c r="G109" s="14">
@@ -3945,7 +3970,7 @@
       <c r="E110" s="26">
         <v>42737</v>
       </c>
-      <c r="F110" s="54">
+      <c r="F110" s="52">
         <v>1</v>
       </c>
       <c r="G110" s="14">
@@ -3963,7 +3988,7 @@
       <c r="E111" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F111" s="54">
+      <c r="F111" s="52">
         <v>1</v>
       </c>
       <c r="G111" s="14">
@@ -3981,7 +4006,7 @@
       <c r="E112" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F112" s="54">
+      <c r="F112" s="52">
         <v>1</v>
       </c>
       <c r="G112" s="14">
@@ -4001,7 +4026,7 @@
       <c r="E113" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F113" s="55">
+      <c r="F113" s="53">
         <v>1</v>
       </c>
       <c r="G113" s="14">
@@ -4021,7 +4046,7 @@
       <c r="E114" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F114" s="55">
+      <c r="F114" s="53">
         <v>1</v>
       </c>
       <c r="G114" s="14">
@@ -4035,7 +4060,7 @@
       <c r="C115" s="19"/>
       <c r="D115" s="19"/>
       <c r="E115" s="19"/>
-      <c r="F115" s="56"/>
+      <c r="F115" s="54"/>
       <c r="G115" s="20"/>
       <c r="H115" s="20"/>
     </row>
@@ -4045,7 +4070,7 @@
       <c r="C116" s="19"/>
       <c r="D116" s="19"/>
       <c r="E116" s="19"/>
-      <c r="F116" s="56"/>
+      <c r="F116" s="54"/>
       <c r="G116" s="20"/>
       <c r="H116" s="20"/>
     </row>
@@ -4055,7 +4080,7 @@
       <c r="C117" s="19"/>
       <c r="D117" s="19"/>
       <c r="E117" s="19"/>
-      <c r="F117" s="56"/>
+      <c r="F117" s="54"/>
       <c r="G117" s="20"/>
       <c r="H117" s="20"/>
     </row>
@@ -4065,7 +4090,7 @@
       <c r="C118" s="19"/>
       <c r="D118" s="19"/>
       <c r="E118" s="19"/>
-      <c r="F118" s="56"/>
+      <c r="F118" s="54"/>
       <c r="G118" s="20"/>
       <c r="H118" s="20"/>
     </row>
@@ -4075,7 +4100,7 @@
       <c r="C119" s="19"/>
       <c r="D119" s="19"/>
       <c r="E119" s="19"/>
-      <c r="F119" s="56"/>
+      <c r="F119" s="54"/>
       <c r="G119" s="20"/>
       <c r="H119" s="20"/>
     </row>
@@ -4085,7 +4110,7 @@
       <c r="C120" s="19"/>
       <c r="D120" s="19"/>
       <c r="E120" s="19"/>
-      <c r="F120" s="56"/>
+      <c r="F120" s="54"/>
       <c r="G120" s="20"/>
       <c r="H120" s="20"/>
     </row>
@@ -4095,7 +4120,7 @@
       <c r="C121" s="19"/>
       <c r="D121" s="19"/>
       <c r="E121" s="19"/>
-      <c r="F121" s="56"/>
+      <c r="F121" s="54"/>
       <c r="G121" s="20"/>
       <c r="H121" s="20"/>
     </row>
@@ -4105,7 +4130,7 @@
       <c r="C122" s="19"/>
       <c r="D122" s="19"/>
       <c r="E122" s="19"/>
-      <c r="F122" s="56"/>
+      <c r="F122" s="54"/>
       <c r="G122" s="20"/>
       <c r="H122" s="20"/>
     </row>
@@ -4115,7 +4140,7 @@
       <c r="C123" s="19"/>
       <c r="D123" s="19"/>
       <c r="E123" s="19"/>
-      <c r="F123" s="56"/>
+      <c r="F123" s="54"/>
       <c r="G123" s="20"/>
       <c r="H123" s="20"/>
     </row>
@@ -4125,7 +4150,7 @@
       <c r="C124" s="19"/>
       <c r="D124" s="19"/>
       <c r="E124" s="19"/>
-      <c r="F124" s="56"/>
+      <c r="F124" s="54"/>
       <c r="G124" s="20"/>
       <c r="H124" s="20"/>
     </row>
@@ -4135,7 +4160,7 @@
       <c r="C125" s="19"/>
       <c r="D125" s="19"/>
       <c r="E125" s="19"/>
-      <c r="F125" s="56"/>
+      <c r="F125" s="54"/>
       <c r="G125" s="20"/>
       <c r="H125" s="20"/>
     </row>
@@ -4145,7 +4170,7 @@
       <c r="C126" s="19"/>
       <c r="D126" s="19"/>
       <c r="E126" s="19"/>
-      <c r="F126" s="56"/>
+      <c r="F126" s="54"/>
       <c r="G126" s="20"/>
       <c r="H126" s="20"/>
     </row>
@@ -4155,7 +4180,7 @@
       <c r="C127" s="19"/>
       <c r="D127" s="19"/>
       <c r="E127" s="19"/>
-      <c r="F127" s="56"/>
+      <c r="F127" s="54"/>
       <c r="G127" s="20"/>
       <c r="H127" s="20"/>
     </row>
@@ -4165,7 +4190,7 @@
       <c r="C128" s="19"/>
       <c r="D128" s="19"/>
       <c r="E128" s="19"/>
-      <c r="F128" s="56"/>
+      <c r="F128" s="54"/>
       <c r="G128" s="20"/>
       <c r="H128" s="20"/>
     </row>
@@ -4175,7 +4200,7 @@
       <c r="C129" s="19"/>
       <c r="D129" s="19"/>
       <c r="E129" s="19"/>
-      <c r="F129" s="56"/>
+      <c r="F129" s="54"/>
       <c r="G129" s="20"/>
       <c r="H129" s="20"/>
     </row>
@@ -4185,7 +4210,7 @@
       <c r="C130" s="19"/>
       <c r="D130" s="19"/>
       <c r="E130" s="19"/>
-      <c r="F130" s="56"/>
+      <c r="F130" s="54"/>
       <c r="G130" s="20"/>
       <c r="H130" s="20"/>
     </row>
@@ -4195,7 +4220,7 @@
       <c r="C131" s="19"/>
       <c r="D131" s="19"/>
       <c r="E131" s="19"/>
-      <c r="F131" s="56"/>
+      <c r="F131" s="54"/>
       <c r="G131" s="20"/>
       <c r="H131" s="20"/>
     </row>
@@ -4205,7 +4230,7 @@
       <c r="C132" s="19"/>
       <c r="D132" s="19"/>
       <c r="E132" s="19"/>
-      <c r="F132" s="56"/>
+      <c r="F132" s="54"/>
       <c r="G132" s="20"/>
       <c r="H132" s="20"/>
     </row>
@@ -4215,7 +4240,7 @@
       <c r="C133" s="19"/>
       <c r="D133" s="19"/>
       <c r="E133" s="19"/>
-      <c r="F133" s="56"/>
+      <c r="F133" s="54"/>
       <c r="G133" s="20"/>
       <c r="H133" s="20"/>
     </row>
@@ -4225,7 +4250,7 @@
       <c r="C134" s="19"/>
       <c r="D134" s="19"/>
       <c r="E134" s="19"/>
-      <c r="F134" s="56"/>
+      <c r="F134" s="54"/>
       <c r="G134" s="20"/>
       <c r="H134" s="20"/>
     </row>
@@ -4235,7 +4260,7 @@
       <c r="C135" s="19"/>
       <c r="D135" s="19"/>
       <c r="E135" s="19"/>
-      <c r="F135" s="56"/>
+      <c r="F135" s="54"/>
       <c r="G135" s="20"/>
       <c r="H135" s="20"/>
     </row>
@@ -4245,7 +4270,7 @@
       <c r="C136" s="19"/>
       <c r="D136" s="19"/>
       <c r="E136" s="19"/>
-      <c r="F136" s="56"/>
+      <c r="F136" s="54"/>
       <c r="G136" s="20"/>
       <c r="H136" s="20"/>
     </row>
@@ -4255,7 +4280,7 @@
       <c r="C137" s="19"/>
       <c r="D137" s="19"/>
       <c r="E137" s="19"/>
-      <c r="F137" s="56"/>
+      <c r="F137" s="54"/>
       <c r="G137" s="20"/>
       <c r="H137" s="20"/>
     </row>
@@ -4265,7 +4290,7 @@
       <c r="C138" s="19"/>
       <c r="D138" s="19"/>
       <c r="E138" s="19"/>
-      <c r="F138" s="56"/>
+      <c r="F138" s="54"/>
       <c r="G138" s="20"/>
       <c r="H138" s="20"/>
     </row>
@@ -4275,7 +4300,7 @@
       <c r="C139" s="19"/>
       <c r="D139" s="19"/>
       <c r="E139" s="19"/>
-      <c r="F139" s="56"/>
+      <c r="F139" s="54"/>
       <c r="G139" s="20"/>
       <c r="H139" s="20"/>
     </row>
@@ -4285,7 +4310,7 @@
       <c r="C140" s="19"/>
       <c r="D140" s="19"/>
       <c r="E140" s="19"/>
-      <c r="F140" s="56"/>
+      <c r="F140" s="54"/>
       <c r="G140" s="20"/>
       <c r="H140" s="20"/>
     </row>
@@ -4295,7 +4320,7 @@
       <c r="C141" s="19"/>
       <c r="D141" s="19"/>
       <c r="E141" s="19"/>
-      <c r="F141" s="56"/>
+      <c r="F141" s="54"/>
       <c r="G141" s="20"/>
       <c r="H141" s="20"/>
     </row>
@@ -4305,7 +4330,7 @@
       <c r="C142" s="19"/>
       <c r="D142" s="19"/>
       <c r="E142" s="19"/>
-      <c r="F142" s="56"/>
+      <c r="F142" s="54"/>
       <c r="G142" s="20"/>
       <c r="H142" s="20"/>
     </row>
@@ -4315,7 +4340,7 @@
       <c r="C143" s="19"/>
       <c r="D143" s="19"/>
       <c r="E143" s="19"/>
-      <c r="F143" s="56"/>
+      <c r="F143" s="54"/>
       <c r="G143" s="20"/>
       <c r="H143" s="20"/>
     </row>
@@ -4325,7 +4350,7 @@
       <c r="C144" s="19"/>
       <c r="D144" s="19"/>
       <c r="E144" s="19"/>
-      <c r="F144" s="56"/>
+      <c r="F144" s="54"/>
       <c r="G144" s="20"/>
       <c r="H144" s="20"/>
     </row>
@@ -4335,7 +4360,7 @@
       <c r="C145" s="19"/>
       <c r="D145" s="19"/>
       <c r="E145" s="19"/>
-      <c r="F145" s="56"/>
+      <c r="F145" s="54"/>
       <c r="G145" s="20"/>
       <c r="H145" s="20"/>
     </row>
@@ -4345,7 +4370,7 @@
       <c r="C146" s="19"/>
       <c r="D146" s="19"/>
       <c r="E146" s="19"/>
-      <c r="F146" s="56"/>
+      <c r="F146" s="54"/>
       <c r="G146" s="20"/>
       <c r="H146" s="20"/>
     </row>
@@ -4355,7 +4380,7 @@
       <c r="C147" s="19"/>
       <c r="D147" s="19"/>
       <c r="E147" s="19"/>
-      <c r="F147" s="56"/>
+      <c r="F147" s="54"/>
       <c r="G147" s="20"/>
       <c r="H147" s="20"/>
     </row>
@@ -4365,7 +4390,7 @@
       <c r="C148" s="19"/>
       <c r="D148" s="19"/>
       <c r="E148" s="19"/>
-      <c r="F148" s="56"/>
+      <c r="F148" s="54"/>
       <c r="G148" s="20"/>
       <c r="H148" s="20"/>
     </row>
@@ -4375,7 +4400,7 @@
       <c r="C149" s="19"/>
       <c r="D149" s="19"/>
       <c r="E149" s="19"/>
-      <c r="F149" s="56"/>
+      <c r="F149" s="54"/>
       <c r="G149" s="20"/>
       <c r="H149" s="20"/>
     </row>
@@ -4385,7 +4410,7 @@
       <c r="C150" s="19"/>
       <c r="D150" s="19"/>
       <c r="E150" s="19"/>
-      <c r="F150" s="56"/>
+      <c r="F150" s="54"/>
       <c r="G150" s="20"/>
       <c r="H150" s="20"/>
     </row>
@@ -4395,7 +4420,7 @@
       <c r="C151" s="19"/>
       <c r="D151" s="19"/>
       <c r="E151" s="19"/>
-      <c r="F151" s="56"/>
+      <c r="F151" s="54"/>
       <c r="G151" s="20"/>
       <c r="H151" s="20"/>
     </row>
@@ -4405,7 +4430,7 @@
       <c r="C152" s="19"/>
       <c r="D152" s="19"/>
       <c r="E152" s="19"/>
-      <c r="F152" s="56"/>
+      <c r="F152" s="54"/>
       <c r="G152" s="20"/>
       <c r="H152" s="20"/>
     </row>
@@ -4415,7 +4440,7 @@
       <c r="C153" s="19"/>
       <c r="D153" s="19"/>
       <c r="E153" s="19"/>
-      <c r="F153" s="56"/>
+      <c r="F153" s="54"/>
       <c r="G153" s="20"/>
       <c r="H153" s="20"/>
     </row>
@@ -4425,7 +4450,7 @@
       <c r="C154" s="19"/>
       <c r="D154" s="19"/>
       <c r="E154" s="19"/>
-      <c r="F154" s="56"/>
+      <c r="F154" s="54"/>
       <c r="G154" s="20"/>
       <c r="H154" s="20"/>
     </row>
@@ -4435,7 +4460,7 @@
       <c r="C155" s="19"/>
       <c r="D155" s="19"/>
       <c r="E155" s="19"/>
-      <c r="F155" s="56"/>
+      <c r="F155" s="54"/>
       <c r="G155" s="20"/>
       <c r="H155" s="20"/>
     </row>
@@ -4445,7 +4470,7 @@
       <c r="C156" s="19"/>
       <c r="D156" s="19"/>
       <c r="E156" s="19"/>
-      <c r="F156" s="56"/>
+      <c r="F156" s="54"/>
       <c r="G156" s="20"/>
       <c r="H156" s="20"/>
     </row>
@@ -4455,7 +4480,7 @@
       <c r="C157" s="19"/>
       <c r="D157" s="19"/>
       <c r="E157" s="19"/>
-      <c r="F157" s="56"/>
+      <c r="F157" s="54"/>
       <c r="G157" s="20"/>
       <c r="H157" s="20"/>
     </row>
@@ -4465,7 +4490,7 @@
       <c r="C158" s="19"/>
       <c r="D158" s="19"/>
       <c r="E158" s="19"/>
-      <c r="F158" s="56"/>
+      <c r="F158" s="54"/>
       <c r="G158" s="20"/>
       <c r="H158" s="20"/>
     </row>
@@ -4475,7 +4500,7 @@
       <c r="C159" s="19"/>
       <c r="D159" s="19"/>
       <c r="E159" s="19"/>
-      <c r="F159" s="56"/>
+      <c r="F159" s="54"/>
       <c r="G159" s="20"/>
       <c r="H159" s="20"/>
     </row>
@@ -4485,7 +4510,7 @@
       <c r="C160" s="19"/>
       <c r="D160" s="19"/>
       <c r="E160" s="19"/>
-      <c r="F160" s="56"/>
+      <c r="F160" s="54"/>
       <c r="G160" s="20"/>
       <c r="H160" s="20"/>
     </row>
@@ -4495,7 +4520,7 @@
       <c r="C161" s="19"/>
       <c r="D161" s="19"/>
       <c r="E161" s="19"/>
-      <c r="F161" s="56"/>
+      <c r="F161" s="54"/>
       <c r="G161" s="20"/>
       <c r="H161" s="20"/>
     </row>
@@ -4505,7 +4530,7 @@
       <c r="C162" s="19"/>
       <c r="D162" s="19"/>
       <c r="E162" s="19"/>
-      <c r="F162" s="56"/>
+      <c r="F162" s="54"/>
       <c r="G162" s="20"/>
       <c r="H162" s="20"/>
     </row>
@@ -4515,7 +4540,7 @@
       <c r="C163" s="19"/>
       <c r="D163" s="19"/>
       <c r="E163" s="19"/>
-      <c r="F163" s="56"/>
+      <c r="F163" s="54"/>
       <c r="G163" s="20"/>
       <c r="H163" s="20"/>
     </row>
@@ -4525,7 +4550,7 @@
       <c r="C164" s="19"/>
       <c r="D164" s="19"/>
       <c r="E164" s="19"/>
-      <c r="F164" s="56"/>
+      <c r="F164" s="54"/>
       <c r="G164" s="20"/>
       <c r="H164" s="20"/>
     </row>
@@ -4535,7 +4560,7 @@
       <c r="C165" s="19"/>
       <c r="D165" s="19"/>
       <c r="E165" s="19"/>
-      <c r="F165" s="56"/>
+      <c r="F165" s="54"/>
       <c r="G165" s="20"/>
       <c r="H165" s="20"/>
     </row>
@@ -4545,7 +4570,7 @@
       <c r="C166" s="19"/>
       <c r="D166" s="19"/>
       <c r="E166" s="19"/>
-      <c r="F166" s="56"/>
+      <c r="F166" s="54"/>
       <c r="G166" s="20"/>
       <c r="H166" s="20"/>
     </row>
@@ -4555,7 +4580,7 @@
       <c r="C167" s="19"/>
       <c r="D167" s="19"/>
       <c r="E167" s="19"/>
-      <c r="F167" s="56"/>
+      <c r="F167" s="54"/>
       <c r="G167" s="20"/>
       <c r="H167" s="20"/>
     </row>
@@ -4565,7 +4590,7 @@
       <c r="C168" s="19"/>
       <c r="D168" s="19"/>
       <c r="E168" s="19"/>
-      <c r="F168" s="56"/>
+      <c r="F168" s="54"/>
       <c r="G168" s="20"/>
       <c r="H168" s="20"/>
     </row>
@@ -4575,7 +4600,7 @@
       <c r="C169" s="19"/>
       <c r="D169" s="19"/>
       <c r="E169" s="19"/>
-      <c r="F169" s="56"/>
+      <c r="F169" s="54"/>
       <c r="G169" s="20"/>
       <c r="H169" s="20"/>
     </row>
@@ -4585,7 +4610,7 @@
       <c r="C170" s="19"/>
       <c r="D170" s="19"/>
       <c r="E170" s="19"/>
-      <c r="F170" s="56"/>
+      <c r="F170" s="54"/>
       <c r="G170" s="20"/>
       <c r="H170" s="20"/>
     </row>
@@ -4595,7 +4620,7 @@
       <c r="C171" s="19"/>
       <c r="D171" s="19"/>
       <c r="E171" s="19"/>
-      <c r="F171" s="56"/>
+      <c r="F171" s="54"/>
       <c r="G171" s="20"/>
       <c r="H171" s="20"/>
     </row>
@@ -4605,7 +4630,7 @@
       <c r="C172" s="19"/>
       <c r="D172" s="19"/>
       <c r="E172" s="19"/>
-      <c r="F172" s="56"/>
+      <c r="F172" s="54"/>
       <c r="G172" s="20"/>
       <c r="H172" s="20"/>
     </row>
@@ -4615,7 +4640,7 @@
       <c r="C173" s="19"/>
       <c r="D173" s="19"/>
       <c r="E173" s="19"/>
-      <c r="F173" s="56"/>
+      <c r="F173" s="54"/>
       <c r="G173" s="20"/>
       <c r="H173" s="20"/>
     </row>
@@ -4625,7 +4650,7 @@
       <c r="C174" s="19"/>
       <c r="D174" s="19"/>
       <c r="E174" s="19"/>
-      <c r="F174" s="56"/>
+      <c r="F174" s="54"/>
       <c r="G174" s="20"/>
       <c r="H174" s="20"/>
     </row>
@@ -4635,7 +4660,7 @@
       <c r="C175" s="19"/>
       <c r="D175" s="19"/>
       <c r="E175" s="19"/>
-      <c r="F175" s="56"/>
+      <c r="F175" s="54"/>
       <c r="G175" s="20"/>
       <c r="H175" s="20"/>
     </row>
@@ -4645,7 +4670,7 @@
       <c r="C176" s="19"/>
       <c r="D176" s="19"/>
       <c r="E176" s="19"/>
-      <c r="F176" s="56"/>
+      <c r="F176" s="54"/>
       <c r="G176" s="20"/>
       <c r="H176" s="20"/>
     </row>
@@ -4655,7 +4680,7 @@
       <c r="C177" s="19"/>
       <c r="D177" s="19"/>
       <c r="E177" s="19"/>
-      <c r="F177" s="56"/>
+      <c r="F177" s="54"/>
       <c r="G177" s="20"/>
       <c r="H177" s="20"/>
     </row>
@@ -4665,7 +4690,7 @@
       <c r="C178" s="19"/>
       <c r="D178" s="19"/>
       <c r="E178" s="19"/>
-      <c r="F178" s="56"/>
+      <c r="F178" s="54"/>
       <c r="G178" s="20"/>
       <c r="H178" s="20"/>
     </row>
@@ -4675,7 +4700,7 @@
       <c r="C179" s="19"/>
       <c r="D179" s="19"/>
       <c r="E179" s="19"/>
-      <c r="F179" s="56"/>
+      <c r="F179" s="54"/>
       <c r="G179" s="21"/>
       <c r="H179" s="21"/>
     </row>
@@ -4685,7 +4710,7 @@
       <c r="C180" s="19"/>
       <c r="D180" s="19"/>
       <c r="E180" s="19"/>
-      <c r="F180" s="56"/>
+      <c r="F180" s="54"/>
       <c r="G180" s="21"/>
       <c r="H180" s="21"/>
     </row>
@@ -4695,7 +4720,7 @@
       <c r="C181" s="19"/>
       <c r="D181" s="19"/>
       <c r="E181" s="19"/>
-      <c r="F181" s="56"/>
+      <c r="F181" s="54"/>
       <c r="G181" s="21"/>
       <c r="H181" s="21"/>
     </row>
@@ -4705,7 +4730,7 @@
       <c r="C182" s="19"/>
       <c r="D182" s="19"/>
       <c r="E182" s="19"/>
-      <c r="F182" s="56"/>
+      <c r="F182" s="54"/>
       <c r="G182" s="21"/>
       <c r="H182" s="21"/>
     </row>
@@ -4715,7 +4740,7 @@
       <c r="C183" s="19"/>
       <c r="D183" s="19"/>
       <c r="E183" s="19"/>
-      <c r="F183" s="56"/>
+      <c r="F183" s="54"/>
       <c r="G183" s="21"/>
       <c r="H183" s="21"/>
     </row>
@@ -4725,7 +4750,7 @@
       <c r="C184" s="19"/>
       <c r="D184" s="19"/>
       <c r="E184" s="19"/>
-      <c r="F184" s="56"/>
+      <c r="F184" s="54"/>
       <c r="G184" s="21"/>
       <c r="H184" s="21"/>
     </row>
@@ -4735,7 +4760,7 @@
       <c r="C185" s="19"/>
       <c r="D185" s="19"/>
       <c r="E185" s="19"/>
-      <c r="F185" s="56"/>
+      <c r="F185" s="54"/>
       <c r="G185" s="21"/>
       <c r="H185" s="21"/>
     </row>
@@ -4745,7 +4770,7 @@
       <c r="C186" s="19"/>
       <c r="D186" s="19"/>
       <c r="E186" s="19"/>
-      <c r="F186" s="56"/>
+      <c r="F186" s="54"/>
       <c r="G186" s="21"/>
       <c r="H186" s="21"/>
     </row>
@@ -4755,7 +4780,7 @@
       <c r="C187" s="19"/>
       <c r="D187" s="19"/>
       <c r="E187" s="19"/>
-      <c r="F187" s="56"/>
+      <c r="F187" s="54"/>
       <c r="G187" s="21"/>
       <c r="H187" s="21"/>
     </row>
@@ -4765,7 +4790,7 @@
       <c r="C188" s="19"/>
       <c r="D188" s="19"/>
       <c r="E188" s="19"/>
-      <c r="F188" s="56"/>
+      <c r="F188" s="54"/>
       <c r="G188" s="21"/>
       <c r="H188" s="21"/>
     </row>
@@ -4775,7 +4800,7 @@
       <c r="C189" s="19"/>
       <c r="D189" s="19"/>
       <c r="E189" s="19"/>
-      <c r="F189" s="56"/>
+      <c r="F189" s="54"/>
       <c r="G189" s="21"/>
       <c r="H189" s="21"/>
     </row>
@@ -4785,7 +4810,7 @@
       <c r="C190" s="19"/>
       <c r="D190" s="19"/>
       <c r="E190" s="19"/>
-      <c r="F190" s="56"/>
+      <c r="F190" s="54"/>
       <c r="G190" s="21"/>
       <c r="H190" s="21"/>
     </row>
@@ -4795,7 +4820,7 @@
       <c r="C191" s="19"/>
       <c r="D191" s="19"/>
       <c r="E191" s="19"/>
-      <c r="F191" s="56"/>
+      <c r="F191" s="54"/>
       <c r="G191" s="21"/>
       <c r="H191" s="21"/>
     </row>
@@ -4805,7 +4830,7 @@
       <c r="C192" s="19"/>
       <c r="D192" s="19"/>
       <c r="E192" s="19"/>
-      <c r="F192" s="56"/>
+      <c r="F192" s="54"/>
       <c r="G192" s="21"/>
       <c r="H192" s="21"/>
     </row>
@@ -4815,7 +4840,7 @@
       <c r="C193" s="19"/>
       <c r="D193" s="19"/>
       <c r="E193" s="19"/>
-      <c r="F193" s="56"/>
+      <c r="F193" s="54"/>
       <c r="G193" s="21"/>
       <c r="H193" s="21"/>
     </row>
@@ -4825,7 +4850,7 @@
       <c r="C194" s="19"/>
       <c r="D194" s="19"/>
       <c r="E194" s="19"/>
-      <c r="F194" s="56"/>
+      <c r="F194" s="54"/>
       <c r="G194" s="21"/>
       <c r="H194" s="21"/>
     </row>
@@ -4835,7 +4860,7 @@
       <c r="C195" s="19"/>
       <c r="D195" s="19"/>
       <c r="E195" s="19"/>
-      <c r="F195" s="56"/>
+      <c r="F195" s="54"/>
       <c r="G195" s="21"/>
       <c r="H195" s="21"/>
     </row>
@@ -4845,7 +4870,7 @@
       <c r="C196" s="19"/>
       <c r="D196" s="19"/>
       <c r="E196" s="19"/>
-      <c r="F196" s="56"/>
+      <c r="F196" s="54"/>
       <c r="G196" s="21"/>
       <c r="H196" s="21"/>
     </row>
@@ -4855,7 +4880,7 @@
       <c r="C197" s="19"/>
       <c r="D197" s="19"/>
       <c r="E197" s="19"/>
-      <c r="F197" s="56"/>
+      <c r="F197" s="54"/>
       <c r="G197" s="21"/>
       <c r="H197" s="21"/>
     </row>
@@ -4865,7 +4890,7 @@
       <c r="C198" s="19"/>
       <c r="D198" s="19"/>
       <c r="E198" s="19"/>
-      <c r="F198" s="56"/>
+      <c r="F198" s="54"/>
       <c r="G198" s="21"/>
       <c r="H198" s="21"/>
     </row>
@@ -4875,7 +4900,7 @@
       <c r="C199" s="19"/>
       <c r="D199" s="19"/>
       <c r="E199" s="19"/>
-      <c r="F199" s="56"/>
+      <c r="F199" s="54"/>
       <c r="G199" s="21"/>
       <c r="H199" s="21"/>
     </row>
@@ -4885,7 +4910,7 @@
       <c r="C200" s="19"/>
       <c r="D200" s="19"/>
       <c r="E200" s="19"/>
-      <c r="F200" s="56"/>
+      <c r="F200" s="54"/>
       <c r="G200" s="21"/>
       <c r="H200" s="21"/>
     </row>
@@ -4895,7 +4920,7 @@
       <c r="C201" s="19"/>
       <c r="D201" s="19"/>
       <c r="E201" s="19"/>
-      <c r="F201" s="56"/>
+      <c r="F201" s="54"/>
       <c r="G201" s="21"/>
       <c r="H201" s="21"/>
     </row>
@@ -4905,7 +4930,7 @@
       <c r="C202" s="19"/>
       <c r="D202" s="19"/>
       <c r="E202" s="19"/>
-      <c r="F202" s="56"/>
+      <c r="F202" s="54"/>
       <c r="G202" s="21"/>
       <c r="H202" s="21"/>
     </row>
@@ -4915,7 +4940,7 @@
       <c r="C203" s="19"/>
       <c r="D203" s="19"/>
       <c r="E203" s="19"/>
-      <c r="F203" s="56"/>
+      <c r="F203" s="54"/>
       <c r="G203" s="21"/>
       <c r="H203" s="21"/>
     </row>
@@ -4925,7 +4950,7 @@
       <c r="C204" s="19"/>
       <c r="D204" s="19"/>
       <c r="E204" s="19"/>
-      <c r="F204" s="56"/>
+      <c r="F204" s="54"/>
       <c r="G204" s="21"/>
       <c r="H204" s="21"/>
     </row>
@@ -4935,7 +4960,7 @@
       <c r="C205" s="19"/>
       <c r="D205" s="19"/>
       <c r="E205" s="19"/>
-      <c r="F205" s="56"/>
+      <c r="F205" s="54"/>
       <c r="G205" s="21"/>
       <c r="H205" s="21"/>
     </row>
@@ -4945,7 +4970,7 @@
       <c r="C206" s="19"/>
       <c r="D206" s="19"/>
       <c r="E206" s="19"/>
-      <c r="F206" s="56"/>
+      <c r="F206" s="54"/>
       <c r="G206" s="21"/>
       <c r="H206" s="21"/>
     </row>
@@ -4955,7 +4980,7 @@
       <c r="C207" s="19"/>
       <c r="D207" s="19"/>
       <c r="E207" s="19"/>
-      <c r="F207" s="56"/>
+      <c r="F207" s="54"/>
       <c r="G207" s="21"/>
       <c r="H207" s="21"/>
     </row>
@@ -4965,7 +4990,7 @@
       <c r="C208" s="19"/>
       <c r="D208" s="19"/>
       <c r="E208" s="19"/>
-      <c r="F208" s="56"/>
+      <c r="F208" s="54"/>
       <c r="G208" s="21"/>
       <c r="H208" s="21"/>
     </row>
@@ -4975,7 +5000,7 @@
       <c r="C209" s="19"/>
       <c r="D209" s="19"/>
       <c r="E209" s="19"/>
-      <c r="F209" s="56"/>
+      <c r="F209" s="54"/>
       <c r="G209" s="21"/>
       <c r="H209" s="21"/>
     </row>
@@ -4985,7 +5010,7 @@
       <c r="C210" s="19"/>
       <c r="D210" s="19"/>
       <c r="E210" s="19"/>
-      <c r="F210" s="56"/>
+      <c r="F210" s="54"/>
       <c r="G210" s="21"/>
       <c r="H210" s="21"/>
     </row>
@@ -4995,7 +5020,7 @@
       <c r="C211" s="19"/>
       <c r="D211" s="19"/>
       <c r="E211" s="19"/>
-      <c r="F211" s="56"/>
+      <c r="F211" s="54"/>
       <c r="G211" s="21"/>
       <c r="H211" s="21"/>
     </row>
@@ -5005,7 +5030,7 @@
       <c r="C212" s="19"/>
       <c r="D212" s="19"/>
       <c r="E212" s="19"/>
-      <c r="F212" s="56"/>
+      <c r="F212" s="54"/>
       <c r="G212" s="21"/>
       <c r="H212" s="21"/>
     </row>
@@ -5015,7 +5040,7 @@
       <c r="C213" s="19"/>
       <c r="D213" s="19"/>
       <c r="E213" s="19"/>
-      <c r="F213" s="56"/>
+      <c r="F213" s="54"/>
       <c r="G213" s="21"/>
       <c r="H213" s="21"/>
     </row>
@@ -5025,7 +5050,7 @@
       <c r="C214" s="19"/>
       <c r="D214" s="19"/>
       <c r="E214" s="19"/>
-      <c r="F214" s="56"/>
+      <c r="F214" s="54"/>
       <c r="G214" s="21"/>
       <c r="H214" s="21"/>
     </row>
@@ -5035,7 +5060,7 @@
       <c r="C215" s="19"/>
       <c r="D215" s="19"/>
       <c r="E215" s="19"/>
-      <c r="F215" s="56"/>
+      <c r="F215" s="54"/>
       <c r="G215" s="21"/>
       <c r="H215" s="21"/>
     </row>
@@ -5045,7 +5070,7 @@
       <c r="C216" s="19"/>
       <c r="D216" s="19"/>
       <c r="E216" s="19"/>
-      <c r="F216" s="56"/>
+      <c r="F216" s="54"/>
       <c r="G216" s="21"/>
       <c r="H216" s="21"/>
     </row>
@@ -5055,7 +5080,7 @@
       <c r="C217" s="19"/>
       <c r="D217" s="19"/>
       <c r="E217" s="19"/>
-      <c r="F217" s="56"/>
+      <c r="F217" s="54"/>
       <c r="G217" s="21"/>
       <c r="H217" s="21"/>
     </row>
@@ -5065,7 +5090,7 @@
       <c r="C218" s="19"/>
       <c r="D218" s="19"/>
       <c r="E218" s="19"/>
-      <c r="F218" s="56"/>
+      <c r="F218" s="54"/>
       <c r="G218" s="21"/>
       <c r="H218" s="21"/>
     </row>
@@ -5075,7 +5100,7 @@
       <c r="C219" s="19"/>
       <c r="D219" s="19"/>
       <c r="E219" s="19"/>
-      <c r="F219" s="56"/>
+      <c r="F219" s="54"/>
       <c r="G219" s="21"/>
       <c r="H219" s="21"/>
     </row>
@@ -5085,7 +5110,7 @@
       <c r="C220" s="19"/>
       <c r="D220" s="19"/>
       <c r="E220" s="19"/>
-      <c r="F220" s="56"/>
+      <c r="F220" s="54"/>
       <c r="G220" s="21"/>
       <c r="H220" s="21"/>
     </row>
@@ -5095,7 +5120,7 @@
       <c r="C221" s="19"/>
       <c r="D221" s="19"/>
       <c r="E221" s="19"/>
-      <c r="F221" s="56"/>
+      <c r="F221" s="54"/>
       <c r="G221" s="21"/>
       <c r="H221" s="21"/>
     </row>
@@ -5105,7 +5130,7 @@
       <c r="C222" s="19"/>
       <c r="D222" s="19"/>
       <c r="E222" s="19"/>
-      <c r="F222" s="56"/>
+      <c r="F222" s="54"/>
       <c r="G222" s="21"/>
       <c r="H222" s="21"/>
     </row>
@@ -5115,7 +5140,7 @@
       <c r="C223" s="19"/>
       <c r="D223" s="19"/>
       <c r="E223" s="19"/>
-      <c r="F223" s="56"/>
+      <c r="F223" s="54"/>
       <c r="G223" s="21"/>
       <c r="H223" s="21"/>
     </row>
@@ -5125,7 +5150,7 @@
       <c r="C224" s="19"/>
       <c r="D224" s="19"/>
       <c r="E224" s="19"/>
-      <c r="F224" s="56"/>
+      <c r="F224" s="54"/>
       <c r="G224" s="21"/>
       <c r="H224" s="21"/>
     </row>
@@ -5135,7 +5160,7 @@
       <c r="C225" s="19"/>
       <c r="D225" s="19"/>
       <c r="E225" s="19"/>
-      <c r="F225" s="56"/>
+      <c r="F225" s="54"/>
       <c r="G225" s="21"/>
       <c r="H225" s="21"/>
     </row>
@@ -5145,7 +5170,7 @@
       <c r="C226" s="19"/>
       <c r="D226" s="19"/>
       <c r="E226" s="19"/>
-      <c r="F226" s="56"/>
+      <c r="F226" s="54"/>
       <c r="G226" s="21"/>
       <c r="H226" s="21"/>
     </row>
@@ -5155,7 +5180,7 @@
       <c r="C227" s="19"/>
       <c r="D227" s="19"/>
       <c r="E227" s="19"/>
-      <c r="F227" s="56"/>
+      <c r="F227" s="54"/>
       <c r="G227" s="21"/>
       <c r="H227" s="21"/>
     </row>
@@ -5165,7 +5190,7 @@
       <c r="C228" s="19"/>
       <c r="D228" s="19"/>
       <c r="E228" s="19"/>
-      <c r="F228" s="56"/>
+      <c r="F228" s="54"/>
       <c r="G228" s="21"/>
       <c r="H228" s="21"/>
     </row>
@@ -5175,7 +5200,7 @@
       <c r="C229" s="19"/>
       <c r="D229" s="19"/>
       <c r="E229" s="19"/>
-      <c r="F229" s="56"/>
+      <c r="F229" s="54"/>
       <c r="G229" s="21"/>
       <c r="H229" s="21"/>
     </row>
@@ -5185,7 +5210,7 @@
       <c r="C230" s="19"/>
       <c r="D230" s="19"/>
       <c r="E230" s="19"/>
-      <c r="F230" s="56"/>
+      <c r="F230" s="54"/>
       <c r="G230" s="21"/>
       <c r="H230" s="21"/>
     </row>
@@ -5195,7 +5220,7 @@
       <c r="C231" s="19"/>
       <c r="D231" s="19"/>
       <c r="E231" s="19"/>
-      <c r="F231" s="56"/>
+      <c r="F231" s="54"/>
       <c r="G231" s="21"/>
       <c r="H231" s="21"/>
     </row>
@@ -5205,7 +5230,7 @@
       <c r="C232" s="19"/>
       <c r="D232" s="19"/>
       <c r="E232" s="19"/>
-      <c r="F232" s="56"/>
+      <c r="F232" s="54"/>
       <c r="G232" s="21"/>
       <c r="H232" s="21"/>
     </row>
@@ -5215,7 +5240,7 @@
       <c r="C233" s="19"/>
       <c r="D233" s="19"/>
       <c r="E233" s="19"/>
-      <c r="F233" s="56"/>
+      <c r="F233" s="54"/>
       <c r="G233" s="21"/>
       <c r="H233" s="21"/>
     </row>
@@ -5225,7 +5250,7 @@
       <c r="C234" s="19"/>
       <c r="D234" s="19"/>
       <c r="E234" s="19"/>
-      <c r="F234" s="56"/>
+      <c r="F234" s="54"/>
       <c r="G234" s="21"/>
       <c r="H234" s="21"/>
     </row>
@@ -5235,7 +5260,7 @@
       <c r="C235" s="19"/>
       <c r="D235" s="19"/>
       <c r="E235" s="19"/>
-      <c r="F235" s="56"/>
+      <c r="F235" s="54"/>
       <c r="G235" s="21"/>
       <c r="H235" s="21"/>
     </row>
@@ -5245,7 +5270,7 @@
       <c r="C236" s="19"/>
       <c r="D236" s="19"/>
       <c r="E236" s="19"/>
-      <c r="F236" s="56"/>
+      <c r="F236" s="54"/>
       <c r="G236" s="21"/>
       <c r="H236" s="21"/>
     </row>
@@ -5255,7 +5280,7 @@
       <c r="C237" s="19"/>
       <c r="D237" s="19"/>
       <c r="E237" s="19"/>
-      <c r="F237" s="56"/>
+      <c r="F237" s="54"/>
       <c r="G237" s="21"/>
       <c r="H237" s="21"/>
     </row>
@@ -5265,7 +5290,7 @@
       <c r="C238" s="19"/>
       <c r="D238" s="19"/>
       <c r="E238" s="19"/>
-      <c r="F238" s="56"/>
+      <c r="F238" s="54"/>
       <c r="G238" s="21"/>
       <c r="H238" s="21"/>
     </row>
@@ -5275,7 +5300,7 @@
       <c r="C239" s="19"/>
       <c r="D239" s="19"/>
       <c r="E239" s="19"/>
-      <c r="F239" s="56"/>
+      <c r="F239" s="54"/>
       <c r="G239" s="21"/>
       <c r="H239" s="21"/>
     </row>
@@ -5285,7 +5310,7 @@
       <c r="C240" s="19"/>
       <c r="D240" s="19"/>
       <c r="E240" s="19"/>
-      <c r="F240" s="56"/>
+      <c r="F240" s="54"/>
       <c r="G240" s="21"/>
       <c r="H240" s="21"/>
     </row>
@@ -5295,7 +5320,7 @@
       <c r="C241" s="19"/>
       <c r="D241" s="19"/>
       <c r="E241" s="19"/>
-      <c r="F241" s="56"/>
+      <c r="F241" s="54"/>
       <c r="G241" s="21"/>
       <c r="H241" s="21"/>
     </row>
@@ -5305,7 +5330,7 @@
       <c r="C242" s="19"/>
       <c r="D242" s="19"/>
       <c r="E242" s="19"/>
-      <c r="F242" s="56"/>
+      <c r="F242" s="54"/>
       <c r="G242" s="21"/>
       <c r="H242" s="21"/>
     </row>
@@ -5315,7 +5340,7 @@
       <c r="C243" s="19"/>
       <c r="D243" s="19"/>
       <c r="E243" s="19"/>
-      <c r="F243" s="56"/>
+      <c r="F243" s="54"/>
       <c r="G243" s="21"/>
       <c r="H243" s="21"/>
     </row>
@@ -5325,7 +5350,7 @@
       <c r="C244" s="19"/>
       <c r="D244" s="19"/>
       <c r="E244" s="19"/>
-      <c r="F244" s="56"/>
+      <c r="F244" s="54"/>
       <c r="G244" s="21"/>
       <c r="H244" s="21"/>
     </row>
@@ -5335,7 +5360,7 @@
       <c r="C245" s="19"/>
       <c r="D245" s="19"/>
       <c r="E245" s="19"/>
-      <c r="F245" s="56"/>
+      <c r="F245" s="54"/>
       <c r="G245" s="21"/>
       <c r="H245" s="21"/>
     </row>
@@ -5345,7 +5370,7 @@
       <c r="C246" s="19"/>
       <c r="D246" s="19"/>
       <c r="E246" s="19"/>
-      <c r="F246" s="56"/>
+      <c r="F246" s="54"/>
       <c r="G246" s="21"/>
       <c r="H246" s="21"/>
     </row>
@@ -5355,7 +5380,7 @@
       <c r="C247" s="19"/>
       <c r="D247" s="19"/>
       <c r="E247" s="19"/>
-      <c r="F247" s="56"/>
+      <c r="F247" s="54"/>
       <c r="G247" s="21"/>
       <c r="H247" s="21"/>
     </row>
@@ -5365,7 +5390,7 @@
       <c r="C248" s="19"/>
       <c r="D248" s="19"/>
       <c r="E248" s="19"/>
-      <c r="F248" s="56"/>
+      <c r="F248" s="54"/>
       <c r="G248" s="21"/>
       <c r="H248" s="21"/>
     </row>
@@ -5375,7 +5400,7 @@
       <c r="C249" s="19"/>
       <c r="D249" s="19"/>
       <c r="E249" s="19"/>
-      <c r="F249" s="56"/>
+      <c r="F249" s="54"/>
       <c r="G249" s="21"/>
       <c r="H249" s="21"/>
     </row>
@@ -5385,7 +5410,7 @@
       <c r="C250" s="19"/>
       <c r="D250" s="19"/>
       <c r="E250" s="19"/>
-      <c r="F250" s="56"/>
+      <c r="F250" s="54"/>
       <c r="G250" s="21"/>
       <c r="H250" s="21"/>
     </row>
@@ -5395,7 +5420,7 @@
       <c r="C251" s="19"/>
       <c r="D251" s="19"/>
       <c r="E251" s="19"/>
-      <c r="F251" s="56"/>
+      <c r="F251" s="54"/>
       <c r="G251" s="21"/>
       <c r="H251" s="21"/>
     </row>
@@ -5405,7 +5430,7 @@
       <c r="C252" s="19"/>
       <c r="D252" s="19"/>
       <c r="E252" s="19"/>
-      <c r="F252" s="56"/>
+      <c r="F252" s="54"/>
       <c r="G252" s="21"/>
       <c r="H252" s="21"/>
     </row>
@@ -5415,7 +5440,7 @@
       <c r="C253" s="19"/>
       <c r="D253" s="19"/>
       <c r="E253" s="19"/>
-      <c r="F253" s="56"/>
+      <c r="F253" s="54"/>
       <c r="G253" s="21"/>
       <c r="H253" s="21"/>
     </row>
@@ -5425,7 +5450,7 @@
       <c r="C254" s="19"/>
       <c r="D254" s="19"/>
       <c r="E254" s="19"/>
-      <c r="F254" s="56"/>
+      <c r="F254" s="54"/>
       <c r="G254" s="21"/>
       <c r="H254" s="21"/>
     </row>
@@ -5435,7 +5460,7 @@
       <c r="C255" s="19"/>
       <c r="D255" s="19"/>
       <c r="E255" s="19"/>
-      <c r="F255" s="56"/>
+      <c r="F255" s="54"/>
       <c r="G255" s="21"/>
       <c r="H255" s="21"/>
     </row>
@@ -5445,7 +5470,7 @@
       <c r="C256" s="19"/>
       <c r="D256" s="19"/>
       <c r="E256" s="19"/>
-      <c r="F256" s="56"/>
+      <c r="F256" s="54"/>
       <c r="G256" s="21"/>
       <c r="H256" s="21"/>
     </row>
@@ -5455,7 +5480,7 @@
       <c r="C257" s="19"/>
       <c r="D257" s="19"/>
       <c r="E257" s="19"/>
-      <c r="F257" s="56"/>
+      <c r="F257" s="54"/>
       <c r="G257" s="21"/>
       <c r="H257" s="21"/>
     </row>
@@ -5465,7 +5490,7 @@
       <c r="C258" s="19"/>
       <c r="D258" s="19"/>
       <c r="E258" s="19"/>
-      <c r="F258" s="56"/>
+      <c r="F258" s="54"/>
       <c r="G258" s="21"/>
       <c r="H258" s="21"/>
     </row>
@@ -5475,7 +5500,7 @@
       <c r="C259" s="19"/>
       <c r="D259" s="19"/>
       <c r="E259" s="19"/>
-      <c r="F259" s="56"/>
+      <c r="F259" s="54"/>
       <c r="G259" s="21"/>
       <c r="H259" s="21"/>
     </row>
@@ -5485,7 +5510,7 @@
       <c r="C260" s="19"/>
       <c r="D260" s="19"/>
       <c r="E260" s="19"/>
-      <c r="F260" s="56"/>
+      <c r="F260" s="54"/>
       <c r="G260" s="21"/>
       <c r="H260" s="21"/>
     </row>
@@ -5495,7 +5520,7 @@
       <c r="C261" s="19"/>
       <c r="D261" s="19"/>
       <c r="E261" s="19"/>
-      <c r="F261" s="56"/>
+      <c r="F261" s="54"/>
       <c r="G261" s="21"/>
       <c r="H261" s="21"/>
     </row>
@@ -5505,7 +5530,7 @@
       <c r="C262" s="19"/>
       <c r="D262" s="19"/>
       <c r="E262" s="19"/>
-      <c r="F262" s="56"/>
+      <c r="F262" s="54"/>
       <c r="G262" s="21"/>
       <c r="H262" s="21"/>
     </row>
@@ -5515,7 +5540,7 @@
       <c r="C263" s="19"/>
       <c r="D263" s="19"/>
       <c r="E263" s="19"/>
-      <c r="F263" s="56"/>
+      <c r="F263" s="54"/>
       <c r="G263" s="21"/>
       <c r="H263" s="21"/>
     </row>
@@ -5525,7 +5550,7 @@
       <c r="C264" s="19"/>
       <c r="D264" s="19"/>
       <c r="E264" s="19"/>
-      <c r="F264" s="56"/>
+      <c r="F264" s="54"/>
       <c r="G264" s="21"/>
       <c r="H264" s="21"/>
     </row>
@@ -5535,7 +5560,7 @@
       <c r="C265" s="19"/>
       <c r="D265" s="19"/>
       <c r="E265" s="19"/>
-      <c r="F265" s="56"/>
+      <c r="F265" s="54"/>
       <c r="G265" s="21"/>
       <c r="H265" s="21"/>
     </row>
@@ -5545,7 +5570,7 @@
       <c r="C266" s="19"/>
       <c r="D266" s="19"/>
       <c r="E266" s="19"/>
-      <c r="F266" s="56"/>
+      <c r="F266" s="54"/>
       <c r="G266" s="21"/>
       <c r="H266" s="21"/>
     </row>
@@ -5555,7 +5580,7 @@
       <c r="C267" s="19"/>
       <c r="D267" s="19"/>
       <c r="E267" s="19"/>
-      <c r="F267" s="56"/>
+      <c r="F267" s="54"/>
       <c r="G267" s="21"/>
       <c r="H267" s="21"/>
     </row>
@@ -5565,7 +5590,7 @@
       <c r="C268" s="19"/>
       <c r="D268" s="19"/>
       <c r="E268" s="19"/>
-      <c r="F268" s="56"/>
+      <c r="F268" s="54"/>
       <c r="G268" s="21"/>
       <c r="H268" s="21"/>
     </row>
@@ -5575,7 +5600,7 @@
       <c r="C269" s="19"/>
       <c r="D269" s="19"/>
       <c r="E269" s="19"/>
-      <c r="F269" s="56"/>
+      <c r="F269" s="54"/>
       <c r="G269" s="21"/>
       <c r="H269" s="21"/>
     </row>
@@ -5585,7 +5610,7 @@
       <c r="C270" s="19"/>
       <c r="D270" s="19"/>
       <c r="E270" s="19"/>
-      <c r="F270" s="56"/>
+      <c r="F270" s="54"/>
       <c r="G270" s="21"/>
       <c r="H270" s="21"/>
     </row>
@@ -5595,7 +5620,7 @@
       <c r="C271" s="19"/>
       <c r="D271" s="19"/>
       <c r="E271" s="19"/>
-      <c r="F271" s="56"/>
+      <c r="F271" s="54"/>
       <c r="G271" s="21"/>
       <c r="H271" s="21"/>
     </row>
@@ -5605,7 +5630,7 @@
       <c r="C272" s="19"/>
       <c r="D272" s="19"/>
       <c r="E272" s="19"/>
-      <c r="F272" s="56"/>
+      <c r="F272" s="54"/>
       <c r="G272" s="21"/>
       <c r="H272" s="21"/>
     </row>
@@ -5615,7 +5640,7 @@
       <c r="C273" s="19"/>
       <c r="D273" s="19"/>
       <c r="E273" s="19"/>
-      <c r="F273" s="56"/>
+      <c r="F273" s="54"/>
       <c r="G273" s="21"/>
       <c r="H273" s="21"/>
     </row>
@@ -5625,7 +5650,7 @@
       <c r="C274" s="19"/>
       <c r="D274" s="19"/>
       <c r="E274" s="19"/>
-      <c r="F274" s="56"/>
+      <c r="F274" s="54"/>
       <c r="G274" s="21"/>
       <c r="H274" s="21"/>
     </row>
@@ -5635,7 +5660,7 @@
       <c r="C275" s="19"/>
       <c r="D275" s="19"/>
       <c r="E275" s="19"/>
-      <c r="F275" s="56"/>
+      <c r="F275" s="54"/>
       <c r="G275" s="21"/>
       <c r="H275" s="21"/>
     </row>
@@ -5645,7 +5670,7 @@
       <c r="C276" s="19"/>
       <c r="D276" s="19"/>
       <c r="E276" s="19"/>
-      <c r="F276" s="56"/>
+      <c r="F276" s="54"/>
       <c r="G276" s="21"/>
       <c r="H276" s="21"/>
     </row>
@@ -5655,7 +5680,7 @@
       <c r="C277" s="19"/>
       <c r="D277" s="19"/>
       <c r="E277" s="19"/>
-      <c r="F277" s="56"/>
+      <c r="F277" s="54"/>
       <c r="G277" s="21"/>
       <c r="H277" s="21"/>
     </row>
@@ -5665,7 +5690,7 @@
       <c r="C278" s="19"/>
       <c r="D278" s="19"/>
       <c r="E278" s="19"/>
-      <c r="F278" s="56"/>
+      <c r="F278" s="54"/>
       <c r="G278" s="21"/>
       <c r="H278" s="21"/>
     </row>
@@ -5675,7 +5700,7 @@
       <c r="C279" s="19"/>
       <c r="D279" s="19"/>
       <c r="E279" s="19"/>
-      <c r="F279" s="56"/>
+      <c r="F279" s="54"/>
       <c r="G279" s="21"/>
       <c r="H279" s="21"/>
     </row>
@@ -5688,8 +5713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD59"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5705,39 +5730,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63" t="s">
         <v>173</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41" t="s">
+      <c r="G1" s="63"/>
+      <c r="H1" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="Q1" s="65" t="s">
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="Q1" s="62" t="s">
         <v>214</v>
       </c>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="AA1" s="65" t="s">
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="AA1" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
@@ -5767,22 +5792,22 @@
       <c r="I2" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="Q2" s="40" t="s">
+      <c r="Q2" s="63" t="s">
         <v>173</v>
       </c>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="41" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="U2" s="41"/>
-      <c r="V2" s="41"/>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
+      <c r="U2" s="64"/>
+      <c r="V2" s="64"/>
+      <c r="W2" s="64"/>
+      <c r="X2" s="64"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -5794,7 +5819,9 @@
       <c r="C3" s="23">
         <v>42766</v>
       </c>
-      <c r="D3" s="23"/>
+      <c r="D3" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F3" t="s">
         <v>122</v>
       </c>
@@ -5851,7 +5878,9 @@
       <c r="C4" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="38" t="s">
+        <v>218</v>
+      </c>
       <c r="E4" s="37" t="s">
         <v>124</v>
       </c>
@@ -5911,7 +5940,9 @@
       <c r="C5" s="38">
         <v>42766</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="38" t="s">
+        <v>218</v>
+      </c>
       <c r="E5" s="37" t="s">
         <v>124</v>
       </c>
@@ -5983,7 +6014,9 @@
       <c r="C6" s="23">
         <v>42767</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F6" t="s">
         <v>122</v>
       </c>
@@ -6040,7 +6073,9 @@
       <c r="C7" s="23">
         <v>42767</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F7" t="s">
         <v>122</v>
       </c>
@@ -6097,7 +6132,9 @@
       <c r="C8" s="23">
         <v>42765</v>
       </c>
-      <c r="D8" s="23"/>
+      <c r="D8" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F8" t="s">
         <v>122</v>
       </c>
@@ -6154,7 +6191,9 @@
       <c r="C9" s="23">
         <v>42766</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F9" t="s">
         <v>122</v>
       </c>
@@ -6211,7 +6250,9 @@
       <c r="C10" s="23">
         <v>42766</v>
       </c>
-      <c r="D10" s="23"/>
+      <c r="D10" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F10" t="s">
         <v>122</v>
       </c>
@@ -6268,7 +6309,9 @@
       <c r="C11" s="23">
         <v>42766</v>
       </c>
-      <c r="D11" s="23"/>
+      <c r="D11" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F11" t="s">
         <v>122</v>
       </c>
@@ -6325,7 +6368,9 @@
       <c r="C12" s="23">
         <v>43132</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E12" t="s">
         <v>127</v>
       </c>
@@ -6385,7 +6430,9 @@
       <c r="C13" s="23">
         <v>42767</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F13" t="s">
         <v>125</v>
       </c>
@@ -6442,7 +6489,9 @@
       <c r="C14" s="23">
         <v>42767</v>
       </c>
-      <c r="D14" s="23"/>
+      <c r="D14" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F14" t="s">
         <v>125</v>
       </c>
@@ -6499,7 +6548,9 @@
       <c r="C15" s="23">
         <v>42767</v>
       </c>
-      <c r="D15" s="23"/>
+      <c r="D15" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F15" t="s">
         <v>125</v>
       </c>
@@ -6556,7 +6607,9 @@
       <c r="C16" s="23">
         <v>42762</v>
       </c>
-      <c r="D16" s="23"/>
+      <c r="D16" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E16" t="s">
         <v>171</v>
       </c>
@@ -6616,7 +6669,9 @@
       <c r="C17" s="23">
         <v>42762</v>
       </c>
-      <c r="D17" s="23"/>
+      <c r="D17" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F17" t="s">
         <v>128</v>
       </c>
@@ -6673,7 +6728,9 @@
       <c r="C18" s="23">
         <v>42762</v>
       </c>
-      <c r="D18" s="23"/>
+      <c r="D18" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F18" t="s">
         <v>128</v>
       </c>
@@ -6730,7 +6787,9 @@
       <c r="C19" s="23">
         <v>42762</v>
       </c>
-      <c r="D19" s="23"/>
+      <c r="D19" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F19" t="s">
         <v>128</v>
       </c>
@@ -6787,7 +6846,9 @@
       <c r="C20" s="23">
         <v>42762</v>
       </c>
-      <c r="D20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F20" t="s">
         <v>128</v>
       </c>
@@ -6832,7 +6893,9 @@
       <c r="C21" s="23">
         <v>42762</v>
       </c>
-      <c r="D21" s="23"/>
+      <c r="D21" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F21" t="s">
         <v>128</v>
       </c>
@@ -6889,7 +6952,9 @@
       <c r="C22" s="38">
         <v>42762</v>
       </c>
-      <c r="D22" s="38"/>
+      <c r="D22" s="38" t="s">
+        <v>218</v>
+      </c>
       <c r="E22" s="37" t="s">
         <v>129</v>
       </c>
@@ -6937,7 +7002,9 @@
       <c r="C23" s="38">
         <v>42762</v>
       </c>
-      <c r="D23" s="38"/>
+      <c r="D23" s="38" t="s">
+        <v>218</v>
+      </c>
       <c r="E23" s="37" t="s">
         <v>129</v>
       </c>
@@ -6997,7 +7064,9 @@
       <c r="C24" s="23">
         <v>42769</v>
       </c>
-      <c r="D24" s="23"/>
+      <c r="D24" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E24" t="s">
         <v>124</v>
       </c>
@@ -7057,7 +7126,9 @@
       <c r="C25" s="23">
         <v>42769</v>
       </c>
-      <c r="D25" s="23"/>
+      <c r="D25" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E25" t="s">
         <v>124</v>
       </c>
@@ -7117,7 +7188,9 @@
       <c r="C26" s="23">
         <v>42769</v>
       </c>
-      <c r="D26" s="23"/>
+      <c r="D26" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E26" t="s">
         <v>124</v>
       </c>
@@ -7177,7 +7250,9 @@
       <c r="C27" s="23">
         <v>42769</v>
       </c>
-      <c r="D27" s="23"/>
+      <c r="D27" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E27" t="s">
         <v>124</v>
       </c>
@@ -7237,7 +7312,9 @@
       <c r="C28" s="23">
         <v>42763</v>
       </c>
-      <c r="D28" s="23"/>
+      <c r="D28" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E28" t="s">
         <v>171</v>
       </c>
@@ -7297,7 +7374,9 @@
       <c r="C29" s="23">
         <v>42763</v>
       </c>
-      <c r="D29" s="23"/>
+      <c r="D29" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F29" t="s">
         <v>135</v>
       </c>
@@ -7354,7 +7433,9 @@
       <c r="C30" s="23">
         <v>42763</v>
       </c>
-      <c r="D30" s="23"/>
+      <c r="D30" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F30" t="s">
         <v>135</v>
       </c>
@@ -7411,7 +7492,9 @@
       <c r="C31" s="23">
         <v>42763</v>
       </c>
-      <c r="D31" s="23"/>
+      <c r="D31" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F31" t="s">
         <v>135</v>
       </c>
@@ -7468,7 +7551,9 @@
       <c r="C32" s="23">
         <v>42942</v>
       </c>
-      <c r="D32" s="23"/>
+      <c r="D32" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F32" t="s">
         <v>122</v>
       </c>
@@ -7504,7 +7589,9 @@
       <c r="C33" s="23">
         <v>42942</v>
       </c>
-      <c r="D33" s="23"/>
+      <c r="D33" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F33" t="s">
         <v>122</v>
       </c>
@@ -7517,18 +7604,18 @@
       <c r="I33">
         <v>2</v>
       </c>
-      <c r="Q33" s="66" t="s">
+      <c r="Q33" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="R33" s="66"/>
-      <c r="S33" s="66"/>
-      <c r="T33" s="66"/>
-      <c r="U33" s="66" t="s">
+      <c r="R33" s="61"/>
+      <c r="S33" s="61"/>
+      <c r="T33" s="61"/>
+      <c r="U33" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="V33" s="66"/>
-      <c r="W33" s="66"/>
-      <c r="X33" s="66"/>
+      <c r="V33" s="61"/>
+      <c r="W33" s="61"/>
+      <c r="X33" s="61"/>
     </row>
     <row r="34" spans="1:24" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -7540,7 +7627,9 @@
       <c r="C34" s="23">
         <v>42942</v>
       </c>
-      <c r="D34" s="23"/>
+      <c r="D34" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F34" t="s">
         <v>122</v>
       </c>
@@ -7553,18 +7642,18 @@
       <c r="I34">
         <v>2</v>
       </c>
-      <c r="Q34" s="64" t="s">
+      <c r="Q34" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="R34" s="64"/>
-      <c r="S34" s="64"/>
-      <c r="T34" s="64"/>
-      <c r="U34" s="64" t="s">
+      <c r="R34" s="60"/>
+      <c r="S34" s="60"/>
+      <c r="T34" s="60"/>
+      <c r="U34" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="V34" s="64"/>
-      <c r="W34" s="64"/>
-      <c r="X34" s="64"/>
+      <c r="V34" s="60"/>
+      <c r="W34" s="60"/>
+      <c r="X34" s="60"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
@@ -7576,7 +7665,9 @@
       <c r="C35" s="23">
         <v>42942</v>
       </c>
-      <c r="D35" s="23"/>
+      <c r="D35" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F35" t="s">
         <v>122</v>
       </c>
@@ -7589,14 +7680,14 @@
       <c r="I35">
         <v>2</v>
       </c>
-      <c r="Q35" s="64"/>
-      <c r="R35" s="64"/>
-      <c r="S35" s="64"/>
-      <c r="T35" s="64"/>
-      <c r="U35" s="64"/>
-      <c r="V35" s="64"/>
-      <c r="W35" s="64"/>
-      <c r="X35" s="64"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="60"/>
+      <c r="T35" s="60"/>
+      <c r="U35" s="60"/>
+      <c r="V35" s="60"/>
+      <c r="W35" s="60"/>
+      <c r="X35" s="60"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -7608,7 +7699,9 @@
       <c r="C36" s="23">
         <v>42942</v>
       </c>
-      <c r="D36" s="23"/>
+      <c r="D36" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F36" t="s">
         <v>122</v>
       </c>
@@ -7621,14 +7714,14 @@
       <c r="I36">
         <v>2</v>
       </c>
-      <c r="Q36" s="64"/>
-      <c r="R36" s="64"/>
-      <c r="S36" s="64"/>
-      <c r="T36" s="64"/>
-      <c r="U36" s="64"/>
-      <c r="V36" s="64"/>
-      <c r="W36" s="64"/>
-      <c r="X36" s="64"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="60"/>
+      <c r="T36" s="60"/>
+      <c r="U36" s="60"/>
+      <c r="V36" s="60"/>
+      <c r="W36" s="60"/>
+      <c r="X36" s="60"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -7640,7 +7733,9 @@
       <c r="C37" s="23">
         <v>42942</v>
       </c>
-      <c r="D37" s="23"/>
+      <c r="D37" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F37" t="s">
         <v>122</v>
       </c>
@@ -7653,14 +7748,14 @@
       <c r="I37">
         <v>2</v>
       </c>
-      <c r="Q37" s="64"/>
-      <c r="R37" s="64"/>
-      <c r="S37" s="64"/>
-      <c r="T37" s="64"/>
-      <c r="U37" s="64"/>
-      <c r="V37" s="64"/>
-      <c r="W37" s="64"/>
-      <c r="X37" s="64"/>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="60"/>
+      <c r="S37" s="60"/>
+      <c r="T37" s="60"/>
+      <c r="U37" s="60"/>
+      <c r="V37" s="60"/>
+      <c r="W37" s="60"/>
+      <c r="X37" s="60"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -7672,7 +7767,9 @@
       <c r="C38" s="23">
         <v>42942</v>
       </c>
-      <c r="D38" s="23"/>
+      <c r="D38" s="23" t="s">
+        <v>216</v>
+      </c>
       <c r="F38" t="s">
         <v>122</v>
       </c>
@@ -7685,14 +7782,14 @@
       <c r="I38">
         <v>2</v>
       </c>
-      <c r="Q38" s="64"/>
-      <c r="R38" s="64"/>
-      <c r="S38" s="64"/>
-      <c r="T38" s="64"/>
-      <c r="U38" s="64"/>
-      <c r="V38" s="64"/>
-      <c r="W38" s="64"/>
-      <c r="X38" s="64"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="60"/>
+      <c r="S38" s="60"/>
+      <c r="T38" s="60"/>
+      <c r="U38" s="60"/>
+      <c r="V38" s="60"/>
+      <c r="W38" s="60"/>
+      <c r="X38" s="60"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -7704,7 +7801,9 @@
       <c r="C39" s="23">
         <v>42942</v>
       </c>
-      <c r="D39" s="23"/>
+      <c r="D39" s="23" t="s">
+        <v>216</v>
+      </c>
       <c r="F39" t="s">
         <v>122</v>
       </c>
@@ -7728,7 +7827,9 @@
       <c r="C40" s="23">
         <v>42942</v>
       </c>
-      <c r="D40" s="23"/>
+      <c r="D40" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F40" t="s">
         <v>122</v>
       </c>
@@ -7752,7 +7853,9 @@
       <c r="C41" s="23">
         <v>42942</v>
       </c>
-      <c r="D41" s="23"/>
+      <c r="D41" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F41" t="s">
         <v>122</v>
       </c>
@@ -7776,7 +7879,9 @@
       <c r="C42" s="23">
         <v>42942</v>
       </c>
-      <c r="D42" s="23"/>
+      <c r="D42" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F42" t="s">
         <v>122</v>
       </c>
@@ -7800,7 +7905,9 @@
       <c r="C43" s="23">
         <v>42942</v>
       </c>
-      <c r="D43" s="23"/>
+      <c r="D43" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F43" t="s">
         <v>122</v>
       </c>
@@ -7824,7 +7931,9 @@
       <c r="C44" s="23">
         <v>42942</v>
       </c>
-      <c r="D44" s="23"/>
+      <c r="D44" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F44" t="s">
         <v>128</v>
       </c>
@@ -7848,7 +7957,9 @@
       <c r="C45" s="23">
         <v>42942</v>
       </c>
-      <c r="D45" s="23"/>
+      <c r="D45" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F45" t="s">
         <v>128</v>
       </c>
@@ -7872,7 +7983,9 @@
       <c r="C46" s="23">
         <v>42942</v>
       </c>
-      <c r="D46" s="23"/>
+      <c r="D46" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F46" t="s">
         <v>128</v>
       </c>
@@ -7896,7 +8009,9 @@
       <c r="C47" s="23">
         <v>42942</v>
       </c>
-      <c r="D47" s="23"/>
+      <c r="D47" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F47" t="s">
         <v>128</v>
       </c>
@@ -7920,10 +8035,10 @@
       <c r="C48" s="38">
         <v>42942</v>
       </c>
-      <c r="D48" s="38"/>
-      <c r="E48" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="D48" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E48" s="37"/>
       <c r="F48" s="37" t="s">
         <v>128</v>
       </c>
@@ -7947,7 +8062,9 @@
       <c r="C49" s="38">
         <v>42942</v>
       </c>
-      <c r="D49" s="38"/>
+      <c r="D49" s="38" t="s">
+        <v>218</v>
+      </c>
       <c r="E49" s="37" t="s">
         <v>129</v>
       </c>
@@ -7974,7 +8091,9 @@
       <c r="C50" s="23">
         <v>42942</v>
       </c>
-      <c r="D50" s="23"/>
+      <c r="D50" s="23" t="s">
+        <v>218</v>
+      </c>
       <c r="F50" t="s">
         <v>128</v>
       </c>
@@ -7998,7 +8117,9 @@
       <c r="C51" s="23">
         <v>42942</v>
       </c>
-      <c r="D51" s="23"/>
+      <c r="D51" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E51" t="s">
         <v>124</v>
       </c>
@@ -8025,7 +8146,9 @@
       <c r="C52" s="23">
         <v>42942</v>
       </c>
-      <c r="D52" s="23"/>
+      <c r="D52" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E52" t="s">
         <v>124</v>
       </c>
@@ -8052,7 +8175,9 @@
       <c r="C53" s="23">
         <v>42942</v>
       </c>
-      <c r="D53" s="23"/>
+      <c r="D53" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E53" t="s">
         <v>124</v>
       </c>
@@ -8079,7 +8204,9 @@
       <c r="C54" s="23">
         <v>42942</v>
       </c>
-      <c r="D54" s="23"/>
+      <c r="D54" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="E54" t="s">
         <v>124</v>
       </c>
@@ -8106,7 +8233,9 @@
       <c r="C55" s="23">
         <v>42942</v>
       </c>
-      <c r="D55" s="23"/>
+      <c r="D55" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F55" t="s">
         <v>135</v>
       </c>
@@ -8130,7 +8259,9 @@
       <c r="C56" s="23">
         <v>42942</v>
       </c>
-      <c r="D56" s="23"/>
+      <c r="D56" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F56" t="s">
         <v>135</v>
       </c>
@@ -8154,7 +8285,9 @@
       <c r="C57" s="23">
         <v>42942</v>
       </c>
-      <c r="D57" s="23"/>
+      <c r="D57" s="23" t="s">
+        <v>216</v>
+      </c>
       <c r="F57" t="s">
         <v>135</v>
       </c>
@@ -8178,7 +8311,9 @@
       <c r="C58" s="23">
         <v>43307</v>
       </c>
-      <c r="D58" s="23"/>
+      <c r="D58" s="23" t="s">
+        <v>217</v>
+      </c>
       <c r="F58" t="s">
         <v>135</v>
       </c>
@@ -8207,6 +8342,9 @@
     <sortCondition ref="G3:G59"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:K1"/>
     <mergeCell ref="U34:X38"/>
     <mergeCell ref="U33:X33"/>
     <mergeCell ref="Q33:T33"/>
@@ -8215,9 +8353,6 @@
     <mergeCell ref="T2:X2"/>
     <mergeCell ref="Q1:X1"/>
     <mergeCell ref="Q34:T38"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8494,17 +8629,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -8514,7 +8649,7 @@
       <c r="A2" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>176</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -8532,19 +8667,19 @@
       <c r="G2" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="65" t="s">
         <v>199</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="58" t="s">
+      <c r="I2" s="65"/>
+      <c r="J2" s="55" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="43">
         <v>5109.030795002157</v>
       </c>
       <c r="C3" s="36">
@@ -8560,7 +8695,7 @@
       <c r="F3" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="44" t="s">
         <v>53</v>
       </c>
       <c r="H3" t="s">
@@ -8572,15 +8707,15 @@
       <c r="J3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="T3" s="53"/>
+      <c r="L3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="T3" s="51"/>
     </row>
     <row r="4" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="43">
         <v>2416.1764705882356</v>
       </c>
       <c r="C4" s="36">
@@ -8596,7 +8731,7 @@
       <c r="F4" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="44" t="s">
         <v>53</v>
       </c>
       <c r="H4" t="s">
@@ -8608,15 +8743,15 @@
       <c r="J4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="T4" s="53"/>
+      <c r="L4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="T4" s="51"/>
     </row>
     <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="43">
         <v>3642.5463496785806</v>
       </c>
       <c r="C5" s="36">
@@ -8632,7 +8767,7 @@
       <c r="F5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="48">
+      <c r="G5" s="46">
         <v>42737</v>
       </c>
       <c r="H5" s="37" t="s">
@@ -8641,18 +8776,18 @@
       <c r="I5" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="T5" s="53"/>
+      <c r="L5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="T5" s="51"/>
     </row>
     <row r="6" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="43">
         <v>5028.6049581927537</v>
       </c>
       <c r="C6" s="36">
@@ -8668,7 +8803,7 @@
       <c r="F6" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="46">
         <v>42737</v>
       </c>
       <c r="H6" t="s">
@@ -8680,15 +8815,15 @@
       <c r="J6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="T6" s="53"/>
+      <c r="L6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="T6" s="51"/>
     </row>
     <row r="7" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="43">
         <v>5633.9477320163442</v>
       </c>
       <c r="C7" s="36">
@@ -8704,7 +8839,7 @@
       <c r="F7" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="46" t="s">
+      <c r="G7" s="44" t="s">
         <v>51</v>
       </c>
       <c r="H7" t="s">
@@ -8716,15 +8851,15 @@
       <c r="J7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="T7" s="53"/>
+      <c r="L7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="T7" s="51"/>
     </row>
     <row r="8" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="43">
         <v>1003.7593211471367</v>
       </c>
       <c r="C8" s="36">
@@ -8740,7 +8875,7 @@
       <c r="F8" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="44" t="s">
         <v>53</v>
       </c>
       <c r="H8" t="s">
@@ -8752,15 +8887,15 @@
       <c r="J8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="T8" s="53"/>
+      <c r="L8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="T8" s="51"/>
     </row>
     <row r="9" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="43">
         <v>929.25615467050307</v>
       </c>
       <c r="C9" s="36">
@@ -8776,7 +8911,7 @@
       <c r="F9" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="44" t="s">
         <v>53</v>
       </c>
       <c r="H9" t="s">
@@ -8788,15 +8923,15 @@
       <c r="J9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="53"/>
-      <c r="P9" s="53"/>
-      <c r="T9" s="53"/>
+      <c r="L9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="T9" s="51"/>
     </row>
     <row r="10" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="B10" s="45">
+      <c r="B10" s="43">
         <v>5305.3518177594005</v>
       </c>
       <c r="C10" s="36">
@@ -8812,7 +8947,7 @@
       <c r="F10" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="44" t="s">
         <v>53</v>
       </c>
       <c r="H10" t="s">
@@ -8824,15 +8959,15 @@
       <c r="J10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="T10" s="53"/>
+      <c r="L10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="T10" s="51"/>
     </row>
     <row r="11" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="43">
         <v>3103.3186269614207</v>
       </c>
       <c r="C11" s="36">
@@ -8848,7 +8983,7 @@
       <c r="F11" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="48">
+      <c r="G11" s="46">
         <v>42737</v>
       </c>
       <c r="H11" t="s">
@@ -8860,15 +8995,15 @@
       <c r="J11" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="53"/>
-      <c r="P11" s="53"/>
-      <c r="T11" s="53"/>
+      <c r="L11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="T11" s="51"/>
     </row>
     <row r="12" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="43">
         <v>5425.756055190709</v>
       </c>
       <c r="C12" s="36">
@@ -8884,7 +9019,7 @@
       <c r="F12" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="46">
         <v>42737</v>
       </c>
       <c r="H12" t="s">
@@ -8896,15 +9031,15 @@
       <c r="J12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="T12" s="53"/>
+      <c r="L12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="T12" s="51"/>
     </row>
     <row r="13" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="45">
+      <c r="B13" s="43">
         <v>6847.6033388314081</v>
       </c>
       <c r="C13" s="36">
@@ -8920,7 +9055,7 @@
       <c r="F13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="46">
         <v>42737</v>
       </c>
       <c r="H13" s="37" t="s">
@@ -8929,18 +9064,18 @@
       <c r="I13" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="J13" s="43" t="s">
+      <c r="J13" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="53"/>
-      <c r="P13" s="53"/>
-      <c r="T13" s="53"/>
+      <c r="L13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="T13" s="51"/>
     </row>
     <row r="14" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="B14" s="45">
+      <c r="B14" s="43">
         <v>7567.3468908234345</v>
       </c>
       <c r="C14" s="36">
@@ -8956,7 +9091,7 @@
       <c r="F14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="46">
         <v>42737</v>
       </c>
       <c r="H14" t="s">
@@ -8968,15 +9103,15 @@
       <c r="J14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="53"/>
-      <c r="P14" s="53"/>
-      <c r="T14" s="53"/>
+      <c r="L14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="T14" s="51"/>
     </row>
     <row r="15" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="B15" s="45">
+      <c r="B15" s="43">
         <v>2737.8869024063506</v>
       </c>
       <c r="C15" s="36">
@@ -8992,7 +9127,7 @@
       <c r="F15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="46" t="s">
+      <c r="G15" s="44" t="s">
         <v>42</v>
       </c>
       <c r="H15" t="s">
@@ -9004,15 +9139,15 @@
       <c r="J15" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="53"/>
-      <c r="P15" s="53"/>
-      <c r="T15" s="53"/>
+      <c r="L15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="T15" s="51"/>
     </row>
     <row r="16" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="B16" s="45">
+      <c r="B16" s="43">
         <v>3345.1559257678555</v>
       </c>
       <c r="C16" s="36">
@@ -9028,7 +9163,7 @@
       <c r="F16" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="46" t="s">
+      <c r="G16" s="44" t="s">
         <v>42</v>
       </c>
       <c r="H16" t="s">
@@ -9040,15 +9175,15 @@
       <c r="J16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L16" s="53"/>
-      <c r="P16" s="53"/>
-      <c r="T16" s="53"/>
+      <c r="L16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="T16" s="51"/>
     </row>
     <row r="17" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="B17" s="45">
+      <c r="B17" s="43">
         <v>224.60693785874722</v>
       </c>
       <c r="C17" s="36">
@@ -9064,7 +9199,7 @@
       <c r="F17" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="46" t="s">
+      <c r="G17" s="44" t="s">
         <v>42</v>
       </c>
       <c r="H17" t="s">
@@ -9076,15 +9211,15 @@
       <c r="J17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L17" s="53"/>
-      <c r="P17" s="53"/>
-      <c r="T17" s="53"/>
+      <c r="L17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="T17" s="51"/>
     </row>
     <row r="18" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="B18" s="45">
+      <c r="B18" s="43">
         <v>1790.3708037265581</v>
       </c>
       <c r="C18" s="36">
@@ -9100,7 +9235,7 @@
       <c r="F18" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="44" t="s">
         <v>42</v>
       </c>
       <c r="H18" t="s">
@@ -9112,15 +9247,15 @@
       <c r="J18" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="53"/>
-      <c r="P18" s="53"/>
-      <c r="T18" s="53"/>
+      <c r="L18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="T18" s="51"/>
     </row>
     <row r="19" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="45">
+      <c r="B19" s="43">
         <v>4908.087316314316</v>
       </c>
       <c r="C19" s="36">
@@ -9136,7 +9271,7 @@
       <c r="F19" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" s="44" t="s">
         <v>42</v>
       </c>
       <c r="H19" s="37" t="s">
@@ -9145,18 +9280,18 @@
       <c r="I19" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="L19" s="53"/>
-      <c r="P19" s="53"/>
-      <c r="T19" s="53"/>
+      <c r="L19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="T19" s="51"/>
     </row>
     <row r="20" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="45">
+      <c r="B20" s="43">
         <v>4551.3310219192581</v>
       </c>
       <c r="C20" s="36">
@@ -9172,7 +9307,7 @@
       <c r="F20" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="46" t="s">
+      <c r="G20" s="44" t="s">
         <v>42</v>
       </c>
       <c r="H20" s="37" t="s">
@@ -9181,18 +9316,18 @@
       <c r="I20" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J20" s="43" t="s">
+      <c r="J20" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="53"/>
-      <c r="P20" s="53"/>
-      <c r="T20" s="53"/>
+      <c r="L20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="T20" s="51"/>
     </row>
     <row r="21" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="45">
+      <c r="B21" s="43">
         <v>6102.8348936145267</v>
       </c>
       <c r="C21" s="36">
@@ -9205,10 +9340,10 @@
       <c r="E21" s="20">
         <v>60.23949169110459</v>
       </c>
-      <c r="F21" s="49" t="s">
+      <c r="F21" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="50" t="s">
+      <c r="G21" s="48" t="s">
         <v>42</v>
       </c>
       <c r="H21" t="s">
@@ -9220,15 +9355,15 @@
       <c r="J21" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L21" s="53"/>
-      <c r="P21" s="53"/>
-      <c r="T21" s="53"/>
+      <c r="L21" s="51"/>
+      <c r="P21" s="51"/>
+      <c r="T21" s="51"/>
     </row>
     <row r="22" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="B22" s="45">
+      <c r="B22" s="43">
         <v>5204.8290471475539</v>
       </c>
       <c r="C22" s="36">
@@ -9244,7 +9379,7 @@
       <c r="F22" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="48">
+      <c r="G22" s="46">
         <v>42796</v>
       </c>
       <c r="H22" t="s">
@@ -9256,15 +9391,15 @@
       <c r="J22" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="54"/>
-      <c r="P22" s="54"/>
-      <c r="T22" s="54"/>
+      <c r="L22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="T22" s="52"/>
     </row>
     <row r="23" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="45">
+      <c r="B23" s="43">
         <v>7508.6694866315493</v>
       </c>
       <c r="C23" s="36">
@@ -9280,7 +9415,7 @@
       <c r="F23" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="48">
+      <c r="G23" s="46">
         <v>42796</v>
       </c>
       <c r="H23" t="s">
@@ -9292,31 +9427,31 @@
       <c r="J23" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="T23" s="54"/>
+      <c r="L23" s="52"/>
+      <c r="P23" s="52"/>
+      <c r="T23" s="52"/>
     </row>
     <row r="24" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="B24" s="45">
+      <c r="B24" s="43">
         <v>4406.5641398263751</v>
       </c>
-      <c r="C24" s="61">
+      <c r="C24" s="58">
         <f t="shared" si="0"/>
         <v>44.06564139826375</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D24" s="59">
         <v>46.43206256109481</v>
       </c>
       <c r="E24" s="20">
         <v>59.872922776148584</v>
       </c>
-      <c r="F24" s="49" t="s">
+      <c r="F24" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="51">
+      <c r="G24" s="49">
         <v>42796</v>
       </c>
       <c r="H24" t="s">
@@ -9328,15 +9463,15 @@
       <c r="J24" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L24" s="54"/>
-      <c r="P24" s="54"/>
-      <c r="T24" s="54"/>
+      <c r="L24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="T24" s="52"/>
     </row>
     <row r="25" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="B25" s="45">
+      <c r="B25" s="43">
         <v>7605.70655443737</v>
       </c>
       <c r="C25" s="36">
@@ -9352,7 +9487,7 @@
       <c r="F25" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="48">
+      <c r="G25" s="46">
         <v>42796</v>
       </c>
       <c r="H25" t="s">
@@ -9364,15 +9499,15 @@
       <c r="J25" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L25" s="54"/>
-      <c r="P25" s="54"/>
-      <c r="T25" s="54"/>
+      <c r="L25" s="52"/>
+      <c r="P25" s="52"/>
+      <c r="T25" s="52"/>
     </row>
     <row r="26" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="B26" s="45">
+      <c r="B26" s="43">
         <v>7404.0620099387734</v>
       </c>
       <c r="C26" s="36">
@@ -9388,7 +9523,7 @@
       <c r="F26" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="46" t="s">
+      <c r="G26" s="44" t="s">
         <v>37</v>
       </c>
       <c r="H26" t="s">
@@ -9400,22 +9535,22 @@
       <c r="J26" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L26" s="53"/>
-      <c r="P26" s="53"/>
-      <c r="T26" s="53"/>
+      <c r="L26" s="51"/>
+      <c r="P26" s="51"/>
+      <c r="T26" s="51"/>
     </row>
     <row r="27" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="B27" s="45">
+      <c r="B27" s="43">
         <v>5048.7172452853556</v>
       </c>
-      <c r="C27" s="61">
+      <c r="C27" s="58">
         <f t="shared" si="0"/>
         <v>50.487172452853557</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="59">
         <v>55.140961857379772</v>
       </c>
       <c r="E27" s="20">
@@ -9424,7 +9559,7 @@
       <c r="F27" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="46" t="s">
+      <c r="G27" s="44" t="s">
         <v>37</v>
       </c>
       <c r="H27" t="s">
@@ -9436,22 +9571,22 @@
       <c r="J27" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L27" s="53"/>
-      <c r="P27" s="53"/>
-      <c r="T27" s="53"/>
+      <c r="L27" s="51"/>
+      <c r="P27" s="51"/>
+      <c r="T27" s="51"/>
     </row>
     <row r="28" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="B28" s="45">
+      <c r="B28" s="43">
         <v>5604.5751633986911</v>
       </c>
-      <c r="C28" s="61">
+      <c r="C28" s="58">
         <f t="shared" si="0"/>
         <v>56.04575163398691</v>
       </c>
-      <c r="D28" s="62">
+      <c r="D28" s="59">
         <v>58.73410724156993</v>
       </c>
       <c r="E28" s="20">
@@ -9460,7 +9595,7 @@
       <c r="F28" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="46" t="s">
+      <c r="G28" s="44" t="s">
         <v>37</v>
       </c>
       <c r="H28" t="s">
@@ -9472,22 +9607,22 @@
       <c r="J28" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L28" s="53"/>
-      <c r="P28" s="53"/>
-      <c r="T28" s="53"/>
+      <c r="L28" s="51"/>
+      <c r="P28" s="51"/>
+      <c r="T28" s="51"/>
     </row>
     <row r="29" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="B29" s="45">
+      <c r="B29" s="43">
         <v>5626.1916180272065</v>
       </c>
-      <c r="C29" s="61">
+      <c r="C29" s="58">
         <f t="shared" si="0"/>
         <v>56.261916180272067</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="59">
         <v>52.653399668325036</v>
       </c>
       <c r="E29" s="20">
@@ -9496,7 +9631,7 @@
       <c r="F29" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="46" t="s">
+      <c r="G29" s="44" t="s">
         <v>37</v>
       </c>
       <c r="H29" t="s">
@@ -9508,9 +9643,9 @@
       <c r="J29" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L29" s="53"/>
-      <c r="P29" s="53"/>
-      <c r="T29" s="53"/>
+      <c r="L29" s="51"/>
+      <c r="P29" s="51"/>
+      <c r="T29" s="51"/>
     </row>
     <row r="30" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
@@ -9520,10 +9655,10 @@
         <v>29.988944168048647</v>
       </c>
       <c r="E30" s="20"/>
-      <c r="F30" s="49" t="s">
+      <c r="F30" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="50" t="s">
+      <c r="G30" s="48" t="s">
         <v>42</v>
       </c>
       <c r="I30"/>
@@ -9536,15 +9671,15 @@
       <c r="K31" s="23"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="60" t="s">
+      <c r="A32" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
       <c r="H32" s="39"/>
       <c r="I32" s="39"/>
       <c r="J32" s="39"/>
@@ -9553,150 +9688,150 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="63" t="s">
+      <c r="A33" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="63"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="63"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="63"/>
+      <c r="A34" s="66"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="63"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="63"/>
-      <c r="J35" s="63"/>
+      <c r="A35" s="66"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="66"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="63"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="63"/>
+      <c r="A36" s="66"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="66"/>
+      <c r="J36" s="66"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="63"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="63"/>
-      <c r="J37" s="63"/>
+      <c r="A37" s="66"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="66"/>
+      <c r="J37" s="66"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="63"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="63"/>
+      <c r="A38" s="66"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="66"/>
+      <c r="J38" s="66"/>
     </row>
     <row r="39" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="44"/>
+      <c r="A39" s="42"/>
     </row>
     <row r="40" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="44"/>
+      <c r="A40" s="42"/>
     </row>
     <row r="41" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="47"/>
+      <c r="A41" s="45"/>
     </row>
     <row r="42" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="44"/>
+      <c r="A42" s="42"/>
     </row>
     <row r="43" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="44"/>
+      <c r="A43" s="42"/>
     </row>
     <row r="44" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="44"/>
+      <c r="A44" s="42"/>
     </row>
     <row r="45" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="44"/>
+      <c r="A45" s="42"/>
     </row>
     <row r="46" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="44"/>
+      <c r="A46" s="42"/>
     </row>
     <row r="47" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="44"/>
+      <c r="A47" s="42"/>
     </row>
     <row r="48" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="44"/>
+      <c r="A48" s="42"/>
     </row>
     <row r="49" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="44"/>
+      <c r="A49" s="42"/>
       <c r="H49"/>
       <c r="L49" s="19"/>
       <c r="P49" s="19"/>
       <c r="T49" s="19"/>
     </row>
     <row r="50" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="44"/>
+      <c r="A50" s="42"/>
       <c r="L50" s="19"/>
       <c r="P50" s="19"/>
       <c r="T50" s="19"/>
     </row>
     <row r="51" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="44"/>
+      <c r="A51" s="42"/>
       <c r="L51" s="19"/>
       <c r="P51" s="19"/>
       <c r="T51" s="19"/>
     </row>
     <row r="52" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="47"/>
+      <c r="A52" s="45"/>
       <c r="L52" s="19"/>
       <c r="P52" s="19"/>
       <c r="T52" s="19"/>
     </row>
     <row r="53" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="44"/>
+      <c r="A53" s="42"/>
       <c r="H53"/>
       <c r="L53" s="19"/>
       <c r="P53" s="19"/>
       <c r="T53" s="19"/>
     </row>
     <row r="54" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="44"/>
+      <c r="A54" s="42"/>
       <c r="H54"/>
       <c r="L54" s="19"/>
       <c r="P54" s="19"/>
       <c r="T54" s="19"/>
     </row>
     <row r="55" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="44"/>
+      <c r="A55" s="42"/>
       <c r="H55"/>
       <c r="I55"/>
       <c r="L55" s="19"/>
@@ -9704,20 +9839,20 @@
       <c r="T55" s="19"/>
     </row>
     <row r="56" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="44"/>
+      <c r="A56" s="42"/>
       <c r="H56"/>
       <c r="I56"/>
     </row>
     <row r="57" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="44"/>
+      <c r="A57" s="42"/>
       <c r="H57"/>
       <c r="I57"/>
     </row>
     <row r="58" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="44"/>
+      <c r="A58" s="42"/>
     </row>
     <row r="59" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="44"/>
+      <c r="A59" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -10065,4 +10200,678 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08273949-4999-42AC-BB13-FED76DD97358}">
+  <dimension ref="A1:G58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3">
+        <v>2.3519000000000001</v>
+      </c>
+      <c r="E3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="23">
+        <v>42766</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="38">
+        <v>42766</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="23">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="23">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="23">
+        <v>42765</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="23">
+        <v>42766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="23">
+        <v>42766</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="23">
+        <v>42766</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="23">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="23">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="23">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" s="23">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="23">
+        <v>42762</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" t="s">
+        <v>111</v>
+      </c>
+      <c r="G17" s="23">
+        <v>42762</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" s="23">
+        <v>42762</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" s="23">
+        <v>42762</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" t="s">
+        <v>114</v>
+      </c>
+      <c r="G20" s="23">
+        <v>42762</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="23">
+        <v>42762</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E22" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="38">
+        <v>42762</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E23" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="G23" s="38">
+        <v>42762</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" s="23">
+        <v>42769</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="23">
+        <v>42769</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" t="s">
+        <v>133</v>
+      </c>
+      <c r="G26" s="23">
+        <v>42769</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" s="23">
+        <v>42769</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" t="s">
+        <v>118</v>
+      </c>
+      <c r="G28" s="23">
+        <v>42763</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F29" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" s="23">
+        <v>42763</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F30" t="s">
+        <v>120</v>
+      </c>
+      <c r="G30" s="23">
+        <v>42763</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" s="23">
+        <v>42763</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" t="s">
+        <v>110</v>
+      </c>
+      <c r="G32" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" t="s">
+        <v>111</v>
+      </c>
+      <c r="G33" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" t="s">
+        <v>112</v>
+      </c>
+      <c r="G34" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" t="s">
+        <v>113</v>
+      </c>
+      <c r="G35" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>109</v>
+      </c>
+      <c r="F37" t="s">
+        <v>115</v>
+      </c>
+      <c r="G37" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" t="s">
+        <v>116</v>
+      </c>
+      <c r="G38" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>109</v>
+      </c>
+      <c r="F39" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" t="s">
+        <v>118</v>
+      </c>
+      <c r="G40" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41" t="s">
+        <v>119</v>
+      </c>
+      <c r="G41" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>109</v>
+      </c>
+      <c r="F42" t="s">
+        <v>120</v>
+      </c>
+      <c r="G42" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F43" t="s">
+        <v>121</v>
+      </c>
+      <c r="G43" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" t="s">
+        <v>110</v>
+      </c>
+      <c r="G44" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" t="s">
+        <v>111</v>
+      </c>
+      <c r="G45" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" t="s">
+        <v>112</v>
+      </c>
+      <c r="G46" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>136</v>
+      </c>
+      <c r="F47" t="s">
+        <v>113</v>
+      </c>
+      <c r="G47" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E48" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="G48" s="38">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E49" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F49" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="G49" s="38">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" t="s">
+        <v>117</v>
+      </c>
+      <c r="G50" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" t="s">
+        <v>131</v>
+      </c>
+      <c r="G51" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>130</v>
+      </c>
+      <c r="F52" t="s">
+        <v>132</v>
+      </c>
+      <c r="G52" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>130</v>
+      </c>
+      <c r="F53" t="s">
+        <v>133</v>
+      </c>
+      <c r="G53" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>130</v>
+      </c>
+      <c r="F54" t="s">
+        <v>134</v>
+      </c>
+      <c r="G54" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E55" t="s">
+        <v>136</v>
+      </c>
+      <c r="F55" t="s">
+        <v>118</v>
+      </c>
+      <c r="G55" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E56" t="s">
+        <v>136</v>
+      </c>
+      <c r="F56" t="s">
+        <v>119</v>
+      </c>
+      <c r="G56" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E57" t="s">
+        <v>136</v>
+      </c>
+      <c r="F57" t="s">
+        <v>120</v>
+      </c>
+      <c r="G57" s="23">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E58" t="s">
+        <v>136</v>
+      </c>
+      <c r="F58" t="s">
+        <v>121</v>
+      </c>
+      <c r="G58" s="23">
+        <v>43307</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up the soil data to easier look for differences in the soil results from USDM and SUA. Results from CN at TBS has not arrived yet.
</commit_message>
<xml_diff>
--- a/Termites/Soil_Data.xlsx
+++ b/Termites/Soil_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansun\Documents\Master\GitHub__R-stat\AfricanBioServices-Vegetation-and-soils\Termites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5C0E2137-9A01-4A9E-9420-54522CE53A8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{75C0470A-A339-45ED-88B1-FC82F0F898BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUAsoil" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="List of blocks" sheetId="6" r:id="rId5"/>
     <sheet name="Ark1" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -799,9 +799,6 @@
     <t>GRAINED</t>
   </si>
   <si>
-    <t>Samples sent with Marit</t>
-  </si>
-  <si>
     <t>31.2.2017</t>
   </si>
   <si>
@@ -812,6 +809,9 @@
   </si>
   <si>
     <t>gram sent</t>
+  </si>
+  <si>
+    <t>Samples sent for P:N analysis a NMBU</t>
   </si>
 </sst>
 </file>
@@ -1582,12 +1582,6 @@
     <xf numFmtId="0" fontId="36" fillId="26" borderId="0" xfId="46" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="30" fillId="28" borderId="0" xfId="45" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="30" fillId="28" borderId="0" xfId="45" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="26" borderId="0" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1596,6 +1590,12 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="26" borderId="0" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1967,7 +1967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I279"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
@@ -5713,8 +5713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD59"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C58"/>
+    <sheetView topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5730,39 +5730,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="64" t="s">
+      <c r="G1" s="61"/>
+      <c r="H1" s="62" t="s">
         <v>172</v>
       </c>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="Q1" s="62" t="s">
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="Q1" s="60" t="s">
         <v>214</v>
       </c>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="AA1" s="62" t="s">
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="AA1" s="60" t="s">
         <v>215</v>
       </c>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="60"/>
+      <c r="AD1" s="60"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
@@ -5792,22 +5792,22 @@
       <c r="I2" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="Q2" s="63" t="s">
+      <c r="Q2" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="64" t="s">
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="62" t="s">
         <v>172</v>
       </c>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="AA2" s="60"/>
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -7604,18 +7604,18 @@
       <c r="I33">
         <v>2</v>
       </c>
-      <c r="Q33" s="61" t="s">
+      <c r="Q33" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="R33" s="61"/>
-      <c r="S33" s="61"/>
-      <c r="T33" s="61"/>
-      <c r="U33" s="61" t="s">
+      <c r="R33" s="64"/>
+      <c r="S33" s="64"/>
+      <c r="T33" s="64"/>
+      <c r="U33" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="V33" s="61"/>
-      <c r="W33" s="61"/>
-      <c r="X33" s="61"/>
+      <c r="V33" s="64"/>
+      <c r="W33" s="64"/>
+      <c r="X33" s="64"/>
     </row>
     <row r="34" spans="1:24" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -7642,18 +7642,18 @@
       <c r="I34">
         <v>2</v>
       </c>
-      <c r="Q34" s="60" t="s">
+      <c r="Q34" s="63" t="s">
         <v>211</v>
       </c>
-      <c r="R34" s="60"/>
-      <c r="S34" s="60"/>
-      <c r="T34" s="60"/>
-      <c r="U34" s="60" t="s">
+      <c r="R34" s="63"/>
+      <c r="S34" s="63"/>
+      <c r="T34" s="63"/>
+      <c r="U34" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="V34" s="60"/>
-      <c r="W34" s="60"/>
-      <c r="X34" s="60"/>
+      <c r="V34" s="63"/>
+      <c r="W34" s="63"/>
+      <c r="X34" s="63"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
@@ -7680,14 +7680,14 @@
       <c r="I35">
         <v>2</v>
       </c>
-      <c r="Q35" s="60"/>
-      <c r="R35" s="60"/>
-      <c r="S35" s="60"/>
-      <c r="T35" s="60"/>
-      <c r="U35" s="60"/>
-      <c r="V35" s="60"/>
-      <c r="W35" s="60"/>
-      <c r="X35" s="60"/>
+      <c r="Q35" s="63"/>
+      <c r="R35" s="63"/>
+      <c r="S35" s="63"/>
+      <c r="T35" s="63"/>
+      <c r="U35" s="63"/>
+      <c r="V35" s="63"/>
+      <c r="W35" s="63"/>
+      <c r="X35" s="63"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -7714,14 +7714,14 @@
       <c r="I36">
         <v>2</v>
       </c>
-      <c r="Q36" s="60"/>
-      <c r="R36" s="60"/>
-      <c r="S36" s="60"/>
-      <c r="T36" s="60"/>
-      <c r="U36" s="60"/>
-      <c r="V36" s="60"/>
-      <c r="W36" s="60"/>
-      <c r="X36" s="60"/>
+      <c r="Q36" s="63"/>
+      <c r="R36" s="63"/>
+      <c r="S36" s="63"/>
+      <c r="T36" s="63"/>
+      <c r="U36" s="63"/>
+      <c r="V36" s="63"/>
+      <c r="W36" s="63"/>
+      <c r="X36" s="63"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -7748,14 +7748,14 @@
       <c r="I37">
         <v>2</v>
       </c>
-      <c r="Q37" s="60"/>
-      <c r="R37" s="60"/>
-      <c r="S37" s="60"/>
-      <c r="T37" s="60"/>
-      <c r="U37" s="60"/>
-      <c r="V37" s="60"/>
-      <c r="W37" s="60"/>
-      <c r="X37" s="60"/>
+      <c r="Q37" s="63"/>
+      <c r="R37" s="63"/>
+      <c r="S37" s="63"/>
+      <c r="T37" s="63"/>
+      <c r="U37" s="63"/>
+      <c r="V37" s="63"/>
+      <c r="W37" s="63"/>
+      <c r="X37" s="63"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -7782,14 +7782,14 @@
       <c r="I38">
         <v>2</v>
       </c>
-      <c r="Q38" s="60"/>
-      <c r="R38" s="60"/>
-      <c r="S38" s="60"/>
-      <c r="T38" s="60"/>
-      <c r="U38" s="60"/>
-      <c r="V38" s="60"/>
-      <c r="W38" s="60"/>
-      <c r="X38" s="60"/>
+      <c r="Q38" s="63"/>
+      <c r="R38" s="63"/>
+      <c r="S38" s="63"/>
+      <c r="T38" s="63"/>
+      <c r="U38" s="63"/>
+      <c r="V38" s="63"/>
+      <c r="W38" s="63"/>
+      <c r="X38" s="63"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -8629,17 +8629,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="61" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -10206,18 +10206,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08273949-4999-42AC-BB13-FED76DD97358}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -10231,7 +10231,7 @@
         <v>107</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>105</v>
@@ -10245,16 +10245,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" t="s">
         <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D3">
-        <v>2.3519000000000001</v>
+        <v>2.8460000000000001</v>
       </c>
       <c r="E3" t="s">
         <v>122</v>

</xml_diff>